<commit_message>
$GEO FY16,17,18 income statements
</commit_message>
<xml_diff>
--- a/$GEO.xlsx
+++ b/$GEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FAE4AE-F06E-44F6-93B2-0CFAE64464DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA08432-3388-43B8-A148-874E8A49B2B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33000" windowHeight="18900" activeTab="1" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33000" windowHeight="18900" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="137">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -425,16 +425,29 @@
   </si>
   <si>
     <t>Proceeds from Assets held for Sale</t>
+  </si>
+  <si>
+    <t>FCF per Share (TTM)</t>
+  </si>
+  <si>
+    <t>FY16</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>GeoAMEY - Joint Venture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -657,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -724,42 +737,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -784,8 +761,47 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -924,13 +940,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>15875</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>15875</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -1274,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F7E03D-6822-49B4-89BA-170833748021}">
   <dimension ref="A2:S38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1295,24 +1311,24 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="G5" s="44" t="s">
+      <c r="B5" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="G5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="46"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="53"/>
       <c r="S5" s="1" t="s">
         <v>100</v>
       </c>
@@ -1451,7 +1467,7 @@
         <f t="shared" si="0"/>
         <v>Q322</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="37">
         <v>44835</v>
       </c>
       <c r="H11" s="14" t="s">
@@ -1500,6 +1516,9 @@
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
+      <c r="S13" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G14" s="6"/>
@@ -1513,13 +1532,16 @@
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
+      <c r="S14" s="64" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
       <c r="G15" s="6"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -1536,10 +1558,10 @@
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="55"/>
       <c r="G16" s="6"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -1556,10 +1578,10 @@
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="55"/>
       <c r="G17" s="6"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -1576,10 +1598,10 @@
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="55"/>
       <c r="G18" s="6"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -1599,10 +1621,10 @@
       <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="37"/>
+      <c r="D19" s="60"/>
       <c r="G19" s="6"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1642,11 +1664,11 @@
       <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
       <c r="G22" s="7"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -1663,36 +1685,36 @@
       <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="55"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="54">
         <v>1984</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="55"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="41"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
@@ -1710,77 +1732,83 @@
       <c r="B29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="57"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="46"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="61">
         <f>C6/'Financial Model'!M65</f>
         <v>1.3134525743305294</v>
       </c>
-      <c r="D33" s="39"/>
+      <c r="D33" s="62"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="61">
         <f>C8/SUM('Financial Model'!$J$4:$M$4)</f>
         <v>0.63049111681270253</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="62"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="61">
         <f>C12/SUM('Financial Model'!$J$4:$M$4)</f>
         <v>1.4386558517002188</v>
       </c>
-      <c r="D35" s="39"/>
+      <c r="D35" s="62"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="61">
         <f>C6/SUM('Financial Model'!J19:M19)</f>
         <v>18.160052892198532</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="62"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="61">
         <f>C12/SUM('Financial Model'!J18:M18)</f>
         <v>41.35338385846331</v>
       </c>
-      <c r="D37" s="39"/>
+      <c r="D37" s="62"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C29:D29"/>
@@ -1796,12 +1824,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{59EB0977-29E5-6644-B546-70A523E0BB16}"/>
@@ -1814,13 +1836,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7542DCCC-3188-4401-8BD1-CCBA020F892C}">
-  <dimension ref="B1:AF94"/>
+  <dimension ref="B1:AG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K83" sqref="K83:N95"/>
+      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1831,13 +1853,13 @@
     <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="50"/>
-    <col min="15" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="9.140625" style="50"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.140625" style="38"/>
+    <col min="15" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.140625" style="38"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:33" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="19" t="s">
         <v>98</v>
       </c>
@@ -1871,59 +1893,62 @@
       <c r="M1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="39" t="s">
         <v>39</v>
       </c>
       <c r="Q1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="W1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:33" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="21"/>
       <c r="H2" s="25">
         <v>44377</v>
@@ -1943,24 +1968,33 @@
       <c r="M2" s="25">
         <v>44834</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="40" t="s">
         <v>105</v>
       </c>
+      <c r="Q2" s="25">
+        <v>42735</v>
+      </c>
+      <c r="R2" s="25">
+        <v>43100</v>
+      </c>
       <c r="S2" s="25">
+        <v>43465</v>
+      </c>
+      <c r="T2" s="25">
         <v>43830</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="U2" s="25">
+      <c r="V2" s="25">
         <v>44561</v>
       </c>
-      <c r="V2" s="52"/>
-    </row>
-    <row r="3" spans="2:32" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:33" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
       <c r="J3" s="26">
-        <f>U3</f>
+        <f>V3</f>
         <v>44985</v>
       </c>
       <c r="K3" s="26">
@@ -1972,15 +2006,15 @@
       <c r="M3" s="26">
         <v>45226</v>
       </c>
-      <c r="N3" s="53">
+      <c r="N3" s="41">
         <v>44971</v>
       </c>
-      <c r="U3" s="26">
+      <c r="V3" s="26">
         <v>44985</v>
       </c>
-      <c r="V3" s="52"/>
-    </row>
-    <row r="4" spans="2:32" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>69</v>
       </c>
@@ -1994,7 +2028,7 @@
         <v>557.27700000000004</v>
       </c>
       <c r="J4" s="23">
-        <f>U4-SUM(G4:I4)</f>
+        <f>V4-SUM(G4:I4)</f>
         <v>557.53900000000021</v>
       </c>
       <c r="K4" s="23">
@@ -2006,25 +2040,34 @@
       <c r="M4" s="23">
         <v>616.68299999999999</v>
       </c>
-      <c r="N4" s="54">
+      <c r="N4" s="42">
         <f>M4*(1+N23)</f>
         <v>653.68398000000002</v>
       </c>
+      <c r="Q4" s="23">
+        <v>2179.4899999999998</v>
+      </c>
+      <c r="R4" s="23">
+        <v>2263.42</v>
+      </c>
       <c r="S4" s="23">
+        <v>2331.386</v>
+      </c>
+      <c r="T4" s="23">
         <v>2477.922</v>
       </c>
-      <c r="T4" s="23">
+      <c r="U4" s="23">
         <v>2350.098</v>
       </c>
-      <c r="U4" s="23">
+      <c r="V4" s="23">
         <v>2256.6120000000001</v>
       </c>
-      <c r="V4" s="54">
+      <c r="W4" s="42">
         <f>SUM(K4:N4)</f>
         <v>2409.7289799999999</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
@@ -2038,7 +2081,7 @@
         <v>399.9</v>
       </c>
       <c r="J5" s="4">
-        <f>U5-SUM(G5:I5)</f>
+        <f>V5-SUM(G5:I5)</f>
         <v>395.9860000000001</v>
       </c>
       <c r="K5" s="4">
@@ -2050,17 +2093,26 @@
       <c r="M5" s="4">
         <v>436.21</v>
       </c>
+      <c r="Q5" s="4">
+        <v>1650.2809999999999</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1700.4949999999999</v>
+      </c>
       <c r="S5" s="4">
+        <v>1755.7719999999999</v>
+      </c>
+      <c r="T5" s="4">
         <v>1858.0650000000001</v>
       </c>
-      <c r="T5" s="4">
+      <c r="U5" s="4">
         <v>1771.4949999999999</v>
       </c>
-      <c r="U5" s="4">
+      <c r="V5" s="4">
         <v>1629.046</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
@@ -2074,7 +2126,7 @@
         <v>32.883000000000003</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" ref="J6:J17" si="0">U6-SUM(G6:I6)</f>
+        <f t="shared" ref="J6:J17" si="0">V6-SUM(G6:I6)</f>
         <v>34.870999999999981</v>
       </c>
       <c r="K6" s="4">
@@ -2086,17 +2138,26 @@
       <c r="M6" s="4">
         <v>32.33</v>
       </c>
+      <c r="Q6" s="4">
+        <v>114.916</v>
+      </c>
+      <c r="R6" s="4">
+        <v>124.297</v>
+      </c>
       <c r="S6" s="4">
+        <v>126.42400000000001</v>
+      </c>
+      <c r="T6" s="4">
         <v>130.82499999999999</v>
       </c>
-      <c r="T6" s="4">
+      <c r="U6" s="4">
         <v>134.68</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="4">
         <v>135.17699999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
@@ -2122,17 +2183,26 @@
       <c r="M7" s="4">
         <v>50.021999999999998</v>
       </c>
+      <c r="Q7" s="4">
+        <v>148.709</v>
+      </c>
+      <c r="R7" s="4">
+        <v>190.34299999999999</v>
+      </c>
       <c r="S7" s="4">
+        <v>184.51499999999999</v>
+      </c>
+      <c r="T7" s="4">
         <v>185.92500000000001</v>
       </c>
-      <c r="T7" s="4">
+      <c r="U7" s="4">
         <v>193.37200000000001</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <v>204.30600000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:32" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>73</v>
       </c>
@@ -2180,26 +2250,34 @@
         <f>M4-M5-M6-M7</f>
         <v>98.121000000000038</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="43"/>
+      <c r="Q8" s="23">
+        <f t="shared" ref="Q8:V8" si="2">Q4-Q5-Q6-Q7</f>
+        <v>265.58399999999983</v>
+      </c>
       <c r="R8" s="23">
-        <f t="shared" ref="R8:U8" si="2">R4-R5-R6-R7</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>248.28500000000017</v>
       </c>
       <c r="S8" s="23">
         <f t="shared" si="2"/>
-        <v>303.10699999999997</v>
+        <v>264.67500000000007</v>
       </c>
       <c r="T8" s="23">
         <f t="shared" si="2"/>
-        <v>250.55100000000004</v>
+        <v>303.10699999999997</v>
       </c>
       <c r="U8" s="23">
         <f t="shared" si="2"/>
+        <v>250.55100000000004</v>
+      </c>
+      <c r="V8" s="23">
+        <f t="shared" si="2"/>
         <v>288.08299999999997</v>
       </c>
-      <c r="V8" s="55"/>
-    </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="W8" s="43"/>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
@@ -2225,17 +2303,26 @@
       <c r="M9" s="4">
         <v>5.1109999999999998</v>
       </c>
+      <c r="Q9" s="4">
+        <v>28.495999999999999</v>
+      </c>
+      <c r="R9" s="4">
+        <v>51.676000000000002</v>
+      </c>
       <c r="S9" s="4">
+        <v>34.755000000000003</v>
+      </c>
+      <c r="T9" s="4">
         <v>28.934000000000001</v>
       </c>
-      <c r="T9" s="4">
+      <c r="U9" s="4">
         <v>23.071999999999999</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="4">
         <v>24.007000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>75</v>
       </c>
@@ -2261,17 +2348,26 @@
       <c r="M10" s="4">
         <v>46.536999999999999</v>
       </c>
+      <c r="Q10" s="4">
+        <v>128.71799999999999</v>
+      </c>
+      <c r="R10" s="4">
+        <v>148.024</v>
+      </c>
       <c r="S10" s="4">
+        <v>150.10300000000001</v>
+      </c>
+      <c r="T10" s="4">
         <v>151.024</v>
       </c>
-      <c r="T10" s="4">
+      <c r="U10" s="4">
         <v>126.837</v>
       </c>
-      <c r="U10" s="4">
+      <c r="V10" s="4">
         <v>129.46</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>87</v>
       </c>
@@ -2297,17 +2393,26 @@
       <c r="M11" s="4">
         <v>-37.487000000000002</v>
       </c>
+      <c r="Q11" s="4">
+        <v>-15.885</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
       <c r="S11" s="4">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
         <v>-4.7949999999999999</v>
       </c>
-      <c r="T11" s="4">
+      <c r="U11" s="4">
         <v>5.319</v>
       </c>
-      <c r="U11" s="4">
+      <c r="V11" s="4">
         <v>4.6929999999999996</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>76</v>
       </c>
@@ -2333,17 +2438,26 @@
       <c r="M12" s="4">
         <v>29.279</v>
       </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
       <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
         <v>-2.6930000000000001</v>
       </c>
-      <c r="T12" s="4">
+      <c r="U12" s="4">
         <v>-6.8310000000000004</v>
       </c>
-      <c r="U12" s="4">
+      <c r="V12" s="4">
         <v>5.4989999999999997</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>77</v>
       </c>
@@ -2391,24 +2505,32 @@
         <f>M8+M9-M10+M11+M12</f>
         <v>48.487000000000037</v>
       </c>
+      <c r="Q13" s="4">
+        <f t="shared" ref="Q13:V13" si="4">Q8+Q9-Q10+Q11+Q12</f>
+        <v>149.47699999999983</v>
+      </c>
       <c r="R13" s="4">
-        <f t="shared" ref="R13:U13" si="4">R8+R9-R10+R11+R12</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>151.93700000000018</v>
       </c>
       <c r="S13" s="4">
         <f t="shared" si="4"/>
-        <v>173.529</v>
+        <v>149.32700000000006</v>
       </c>
       <c r="T13" s="4">
         <f t="shared" si="4"/>
-        <v>145.27400000000006</v>
+        <v>173.529</v>
       </c>
       <c r="U13" s="4">
         <f t="shared" si="4"/>
+        <v>145.27400000000006</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="4"/>
         <v>192.82199999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2434,17 +2556,26 @@
       <c r="M14" s="4">
         <v>11.246</v>
       </c>
+      <c r="Q14" s="4">
+        <v>7.9039999999999999</v>
+      </c>
+      <c r="R14" s="4">
+        <v>17.957999999999998</v>
+      </c>
       <c r="S14" s="4">
+        <v>14.117000000000001</v>
+      </c>
+      <c r="T14" s="4">
         <v>16.648</v>
       </c>
-      <c r="T14" s="4">
+      <c r="U14" s="4">
         <v>20.463000000000001</v>
       </c>
-      <c r="U14" s="4">
+      <c r="V14" s="4">
         <v>122.73</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>79</v>
       </c>
@@ -2470,17 +2601,26 @@
       <c r="M15" s="4">
         <v>1.071</v>
       </c>
+      <c r="Q15" s="4">
+        <v>6.9249999999999998</v>
+      </c>
+      <c r="R15" s="4">
+        <v>12.045</v>
+      </c>
       <c r="S15" s="4">
+        <v>9.6270000000000007</v>
+      </c>
+      <c r="T15" s="4">
         <v>9.532</v>
       </c>
-      <c r="T15" s="4">
+      <c r="U15" s="4">
         <v>9.1660000000000004</v>
       </c>
-      <c r="U15" s="4">
+      <c r="V15" s="4">
         <v>7.141</v>
       </c>
     </row>
-    <row r="16" spans="2:32" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>80</v>
       </c>
@@ -2528,26 +2668,34 @@
         <f>M13-M14+M15</f>
         <v>38.312000000000033</v>
       </c>
-      <c r="N16" s="55"/>
+      <c r="N16" s="43"/>
+      <c r="Q16" s="23">
+        <f t="shared" ref="Q16:V16" si="6">Q13-Q14+Q15</f>
+        <v>148.49799999999985</v>
+      </c>
       <c r="R16" s="23">
-        <f t="shared" ref="R16:U16" si="6">R13-R14+R15</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>146.02400000000017</v>
       </c>
       <c r="S16" s="23">
         <f t="shared" si="6"/>
-        <v>166.41300000000001</v>
+        <v>144.83700000000007</v>
       </c>
       <c r="T16" s="23">
         <f t="shared" si="6"/>
-        <v>133.97700000000006</v>
+        <v>166.41300000000001</v>
       </c>
       <c r="U16" s="23">
         <f t="shared" si="6"/>
+        <v>133.97700000000006</v>
+      </c>
+      <c r="V16" s="23">
+        <f t="shared" si="6"/>
         <v>77.232999999999976</v>
       </c>
-      <c r="V16" s="55"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="W16" s="43"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>88</v>
       </c>
@@ -2573,17 +2721,26 @@
       <c r="M17" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="Q17" s="4">
+        <v>0.217</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0.217</v>
+      </c>
       <c r="S17" s="4">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="T17" s="4">
         <v>0.191</v>
       </c>
-      <c r="T17" s="4">
+      <c r="U17" s="4">
         <v>0.20100000000000001</v>
       </c>
-      <c r="U17" s="4">
+      <c r="V17" s="4">
         <v>0.185</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>89</v>
       </c>
@@ -2631,71 +2788,91 @@
         <f>M16+M17</f>
         <v>38.337000000000032</v>
       </c>
+      <c r="Q18" s="4">
+        <f t="shared" ref="Q18:V18" si="8">Q16+Q17</f>
+        <v>148.71499999999986</v>
+      </c>
       <c r="R18" s="4">
-        <f t="shared" ref="R18:U18" si="8">R16+R17</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>146.24100000000018</v>
       </c>
       <c r="S18" s="4">
         <f t="shared" si="8"/>
-        <v>166.60400000000001</v>
+        <v>145.09900000000007</v>
       </c>
       <c r="T18" s="4">
         <f t="shared" si="8"/>
-        <v>134.17800000000005</v>
+        <v>166.60400000000001</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="8"/>
+        <v>134.17800000000005</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="8"/>
         <v>77.417999999999978</v>
       </c>
     </row>
-    <row r="19" spans="2:22" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="48" t="s">
+    <row r="19" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="48">
-        <f>G18/G20</f>
+      <c r="G19" s="36">
+        <f t="shared" ref="G19:M19" si="9">G18/G20</f>
         <v>0.42112279415440457</v>
       </c>
-      <c r="H19" s="48">
-        <f>H18/H20</f>
+      <c r="H19" s="36">
+        <f t="shared" si="9"/>
         <v>0.34842143723116237</v>
       </c>
-      <c r="I19" s="48">
-        <f>I18/I20</f>
+      <c r="I19" s="36">
+        <f t="shared" si="9"/>
         <v>0.28799004355942803</v>
       </c>
-      <c r="J19" s="48">
-        <f>J18/J20</f>
+      <c r="J19" s="36">
+        <f t="shared" si="9"/>
         <v>-0.4136347022860174</v>
       </c>
-      <c r="K19" s="48">
-        <f>K18/K20</f>
+      <c r="K19" s="36">
+        <f t="shared" si="9"/>
         <v>0.31660784995940783</v>
       </c>
-      <c r="L19" s="48">
-        <f>L18/L20</f>
+      <c r="L19" s="36">
+        <f t="shared" si="9"/>
         <v>0.44358853689346872</v>
       </c>
-      <c r="M19" s="48">
-        <f>M18/M20</f>
+      <c r="M19" s="36">
+        <f t="shared" si="9"/>
         <v>0.31643197913399501</v>
       </c>
-      <c r="N19" s="56"/>
-      <c r="S19" s="48">
-        <f>S18/S20</f>
+      <c r="N19" s="44"/>
+      <c r="Q19" s="36">
+        <f t="shared" ref="Q19:S19" si="10">Q18/Q20</f>
+        <v>1.3389906811326688</v>
+      </c>
+      <c r="R19" s="36">
+        <f t="shared" si="10"/>
+        <v>1.2177109788084448</v>
+      </c>
+      <c r="S19" s="36">
+        <f t="shared" si="10"/>
+        <v>1.2067348075947479</v>
+      </c>
+      <c r="T19" s="36">
+        <f>T18/T20</f>
         <v>1.3989050849734668</v>
       </c>
-      <c r="T19" s="48">
-        <f>T18/T20</f>
+      <c r="U19" s="36">
+        <f>U18/U20</f>
         <v>1.1207744802412321</v>
       </c>
-      <c r="U19" s="48">
-        <f>U18/U20</f>
+      <c r="V19" s="36">
+        <f>V18/V20</f>
         <v>0.64309210526315774</v>
       </c>
-      <c r="V19" s="56"/>
-    </row>
-    <row r="20" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="44"/>
+    </row>
+    <row r="20" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2886,7 @@
         <v>120.52500000000001</v>
       </c>
       <c r="J20" s="4">
-        <f>U20</f>
+        <f>V20</f>
         <v>120.384</v>
       </c>
       <c r="K20" s="4">
@@ -2721,23 +2898,32 @@
       <c r="M20" s="4">
         <v>121.154</v>
       </c>
-      <c r="N20" s="57"/>
+      <c r="N20" s="45"/>
+      <c r="Q20" s="63">
+        <v>111.065</v>
+      </c>
+      <c r="R20" s="63">
+        <v>120.095</v>
+      </c>
       <c r="S20" s="4">
+        <v>120.241</v>
+      </c>
+      <c r="T20" s="4">
         <v>119.096</v>
       </c>
-      <c r="T20" s="4">
+      <c r="U20" s="4">
         <v>119.71899999999999</v>
       </c>
-      <c r="U20" s="4">
+      <c r="V20" s="4">
         <v>120.384</v>
       </c>
-      <c r="V20" s="57"/>
-    </row>
-    <row r="21" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N21" s="57"/>
-      <c r="V21" s="57"/>
-    </row>
-    <row r="22" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="45"/>
+    </row>
+    <row r="21" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N21" s="45"/>
+      <c r="W21" s="45"/>
+    </row>
+    <row r="22" spans="2:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
         <v>82</v>
       </c>
@@ -2753,26 +2939,38 @@
         <f>M4/I4-1</f>
         <v>0.10660048772872366</v>
       </c>
-      <c r="N22" s="54"/>
+      <c r="N22" s="42"/>
+      <c r="R22" s="28">
+        <f t="shared" ref="R22" si="11">R4/Q4-1</f>
+        <v>3.8509008988341531E-2</v>
+      </c>
+      <c r="S22" s="28">
+        <f t="shared" ref="S22" si="12">S4/R4-1</f>
+        <v>3.0028010709457265E-2</v>
+      </c>
       <c r="T22" s="28">
-        <f t="shared" ref="T22:U22" si="9">T4/S4-1</f>
+        <f t="shared" ref="T22" si="13">T4/S4-1</f>
+        <v>6.2853598674779798E-2</v>
+      </c>
+      <c r="U22" s="28">
+        <f t="shared" ref="U22" si="14">U4/T4-1</f>
         <v>-5.1585158854879243E-2</v>
       </c>
-      <c r="U22" s="28">
-        <f>U4/T4-1</f>
+      <c r="V22" s="28">
+        <f>V4/U4-1</f>
         <v>-3.9779617701048986E-2</v>
       </c>
-      <c r="V22" s="60">
-        <f>V4/U4-1</f>
+      <c r="W22" s="48">
+        <f>W4/V4-1</f>
         <v>6.7852594952078515E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H23" s="30">
-        <f t="shared" ref="H23:I23" si="10">H4/G4-1</f>
+        <f t="shared" ref="H23" si="15">H4/G4-1</f>
         <v>-1.9011862027804693E-2</v>
       </c>
       <c r="I23" s="30">
@@ -2780,52 +2978,58 @@
         <v>-1.4399940575042458E-2</v>
       </c>
       <c r="J23" s="30">
-        <f t="shared" ref="J23:L23" si="11">J4/I4-1</f>
+        <f t="shared" ref="J23:L23" si="16">J4/I4-1</f>
         <v>4.7014321423666239E-4</v>
       </c>
       <c r="K23" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>-1.1396512172243134E-2</v>
       </c>
       <c r="L23" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>6.7113582553952167E-2</v>
       </c>
       <c r="M23" s="30">
         <f>M4/L4-1</f>
         <v>4.8465002881785457E-2</v>
       </c>
-      <c r="N23" s="58">
+      <c r="N23" s="46">
         <v>0.06</v>
       </c>
-      <c r="R23" s="61" t="s">
+      <c r="Q23" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="S23" s="61" t="s">
+      <c r="R23" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="T23" s="61" t="s">
+      <c r="S23" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="U23" s="61" t="s">
+      <c r="T23" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="V23" s="57"/>
-    </row>
-    <row r="24" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N24" s="57"/>
-      <c r="V24" s="57"/>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="U23" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="V23" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="W23" s="45"/>
+    </row>
+    <row r="24" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N24" s="45"/>
+      <c r="W24" s="45"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="30">
-        <f t="shared" ref="G26:H26" si="12">G8/G4</f>
+        <f t="shared" ref="G26" si="17">G8/G4</f>
         <v>0.11386644505245691</v>
       </c>
       <c r="H26" s="30">
-        <f t="shared" ref="H26:I26" si="13">H8/H4</f>
+        <f t="shared" ref="H26" si="18">H8/H4</f>
         <v>0.12807493204154791</v>
       </c>
       <c r="I26" s="30">
@@ -2833,11 +3037,11 @@
         <v>0.1328226357807698</v>
       </c>
       <c r="J26" s="30">
-        <f t="shared" ref="J26:K26" si="14">J8/J4</f>
+        <f t="shared" ref="J26:K26" si="19">J8/J4</f>
         <v>0.13634561887150509</v>
       </c>
       <c r="K26" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0.14791041120494927</v>
       </c>
       <c r="L26" s="30">
@@ -2848,29 +3052,41 @@
         <f>M8/M4</f>
         <v>0.15911092084588035</v>
       </c>
+      <c r="Q26" s="30">
+        <f t="shared" ref="Q26:T26" si="20">Q8/Q4</f>
+        <v>0.12185603053925453</v>
+      </c>
+      <c r="R26" s="30">
+        <f t="shared" si="20"/>
+        <v>0.10969462141361309</v>
+      </c>
       <c r="S26" s="30">
-        <f t="shared" ref="S26:T26" si="15">S8/S4</f>
+        <f t="shared" si="20"/>
+        <v>0.11352688915520642</v>
+      </c>
+      <c r="T26" s="30">
+        <f t="shared" ref="T26" si="21">T8/T4</f>
         <v>0.12232305940219262</v>
-      </c>
-      <c r="T26" s="30">
-        <f>T8/T4</f>
-        <v>0.10661300081954031</v>
       </c>
       <c r="U26" s="30">
         <f>U8/U4</f>
+        <v>0.10661300081954031</v>
+      </c>
+      <c r="V26" s="30">
+        <f>V8/V4</f>
         <v>0.12766173360772695</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G27" s="30">
-        <f t="shared" ref="G27:H27" si="16">G16/G4</f>
+        <f t="shared" ref="G27" si="22">G16/G4</f>
         <v>8.7586770464470221E-2</v>
       </c>
       <c r="H27" s="30">
-        <f t="shared" ref="H27:I27" si="17">H16/H4</f>
+        <f t="shared" ref="H27" si="23">H16/H4</f>
         <v>7.4159163381492241E-2</v>
       </c>
       <c r="I27" s="30">
@@ -2878,11 +3094,11 @@
         <v>6.2161187344893218E-2</v>
       </c>
       <c r="J27" s="30">
-        <f t="shared" ref="J27:K27" si="18">J16/J4</f>
+        <f t="shared" ref="J27:K27" si="24">J16/J4</f>
         <v>-8.9360564911154017E-2</v>
       </c>
       <c r="K27" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>6.9267124468191194E-2</v>
       </c>
       <c r="L27" s="30">
@@ -2893,29 +3109,41 @@
         <f>M16/M4</f>
         <v>6.212592207017225E-2</v>
       </c>
+      <c r="Q27" s="30">
+        <f t="shared" ref="Q27:T27" si="25">Q16/Q4</f>
+        <v>6.8134288296803319E-2</v>
+      </c>
+      <c r="R27" s="30">
+        <f t="shared" si="25"/>
+        <v>6.4514760848627367E-2</v>
+      </c>
       <c r="S27" s="30">
-        <f t="shared" ref="S27:T27" si="19">S16/S4</f>
+        <f t="shared" si="25"/>
+        <v>6.2124847622830402E-2</v>
+      </c>
+      <c r="T27" s="30">
+        <f t="shared" ref="T27" si="26">T16/T4</f>
         <v>6.7158288275417879E-2</v>
-      </c>
-      <c r="T27" s="30">
-        <f>T16/T4</f>
-        <v>5.7009111960437418E-2</v>
       </c>
       <c r="U27" s="30">
         <f>U16/U4</f>
+        <v>5.7009111960437418E-2</v>
+      </c>
+      <c r="V27" s="30">
+        <f>V16/V4</f>
         <v>3.4225201319500194E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G28" s="30">
-        <f t="shared" ref="G28:H28" si="20">G14/G13</f>
+        <f t="shared" ref="G28" si="27">G14/G13</f>
         <v>0.14082157749977833</v>
       </c>
       <c r="H28" s="30">
-        <f t="shared" ref="H28:I28" si="21">H14/H13</f>
+        <f t="shared" ref="H28" si="28">H14/H13</f>
         <v>0.11238124833525712</v>
       </c>
       <c r="I28" s="30">
@@ -2923,11 +3151,11 @@
         <v>0.20279737172673659</v>
       </c>
       <c r="J28" s="30">
-        <f t="shared" ref="J28:K28" si="22">J14/J13</f>
+        <f t="shared" ref="J28:K28" si="29">J14/J13</f>
         <v>2.0259501389471963</v>
       </c>
       <c r="K28" s="30">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>0.32714093177430542</v>
       </c>
       <c r="L28" s="30">
@@ -2938,25 +3166,37 @@
         <f>M14/M13</f>
         <v>0.23193845773093802</v>
       </c>
+      <c r="Q28" s="30">
+        <f t="shared" ref="Q28:T28" si="30">Q14/Q13</f>
+        <v>5.2877700248198781E-2</v>
+      </c>
+      <c r="R28" s="30">
+        <f t="shared" si="30"/>
+        <v>0.11819372503076918</v>
+      </c>
       <c r="S28" s="30">
-        <f t="shared" ref="S28:T28" si="23">S14/S13</f>
+        <f t="shared" si="30"/>
+        <v>9.4537491545400337E-2</v>
+      </c>
+      <c r="T28" s="30">
+        <f t="shared" ref="T28" si="31">T14/T13</f>
         <v>9.5937854767790973E-2</v>
-      </c>
-      <c r="T28" s="30">
-        <f>T14/T13</f>
-        <v>0.14085796494899289</v>
       </c>
       <c r="U28" s="30">
         <f>U14/U13</f>
+        <v>0.14085796494899289</v>
+      </c>
+      <c r="V28" s="30">
+        <f>V14/V13</f>
         <v>0.63649376108535338</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B31" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="2:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
         <v>4</v>
       </c>
@@ -2972,14 +3212,14 @@
       <c r="M32" s="23">
         <v>91.644999999999996</v>
       </c>
-      <c r="N32" s="55"/>
-      <c r="U32" s="23">
+      <c r="N32" s="43"/>
+      <c r="V32" s="23">
         <f>J32</f>
         <v>506.49099999999999</v>
       </c>
-      <c r="V32" s="55"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="W32" s="43"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2995,12 +3235,12 @@
       <c r="M33" s="4">
         <v>0</v>
       </c>
-      <c r="U33" s="4">
+      <c r="V33" s="4">
         <f>J33</f>
         <v>20.161000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
@@ -3016,12 +3256,12 @@
       <c r="M34" s="4">
         <v>383.69400000000002</v>
       </c>
-      <c r="U34" s="4">
-        <f t="shared" ref="U34:U44" si="24">J34</f>
+      <c r="V34" s="4">
+        <f t="shared" ref="V34:V44" si="32">J34</f>
         <v>365.57299999999998</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
@@ -3037,12 +3277,12 @@
       <c r="M35" s="4">
         <v>0</v>
       </c>
-      <c r="U35" s="4">
-        <f t="shared" si="24"/>
+      <c r="V35" s="4">
+        <f t="shared" si="32"/>
         <v>6.5069999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
@@ -3058,81 +3298,89 @@
       <c r="M36" s="4">
         <v>40.387999999999998</v>
       </c>
-      <c r="U36" s="4">
-        <f t="shared" si="24"/>
+      <c r="V36" s="4">
+        <f t="shared" si="32"/>
         <v>45.176000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ref="C37:N37" si="25">SUM(C32:C36)</f>
+        <f t="shared" ref="C37:N37" si="33">SUM(C32:C36)</f>
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>943.90800000000002</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>1022.8150000000001</v>
       </c>
       <c r="L37" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>1023.413</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(M32:M36)</f>
         <v>515.72699999999998</v>
       </c>
-      <c r="N37" s="50">
-        <f t="shared" si="25"/>
+      <c r="N37" s="38">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="4">
+        <f t="shared" ref="Q37:S37" si="34">SUM(Q32:Q36)</f>
         <v>0</v>
       </c>
       <c r="R37" s="4">
-        <f t="shared" ref="R37:U37" si="26">SUM(R32:R36)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="S37" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="S37:V37" si="35">SUM(S32:S36)</f>
         <v>0</v>
       </c>
       <c r="T37" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="U37" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="4">
+        <f t="shared" si="35"/>
         <v>943.90800000000002</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>46</v>
       </c>
@@ -3148,12 +3396,12 @@
       <c r="M38" s="4">
         <v>89.76</v>
       </c>
-      <c r="U38" s="4">
-        <f t="shared" si="24"/>
+      <c r="V38" s="4">
+        <f t="shared" si="32"/>
         <v>76.158000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>66</v>
       </c>
@@ -3169,12 +3417,12 @@
       <c r="M39" s="4">
         <v>2012.6790000000001</v>
       </c>
-      <c r="U39" s="4">
-        <f t="shared" si="24"/>
+      <c r="V39" s="4">
+        <f t="shared" si="32"/>
         <v>2037.845</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
@@ -3190,12 +3438,12 @@
       <c r="M40" s="4">
         <v>0</v>
       </c>
-      <c r="U40" s="4">
-        <f t="shared" si="24"/>
+      <c r="V40" s="4">
+        <f t="shared" si="32"/>
         <v>367.07100000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>47</v>
       </c>
@@ -3211,12 +3459,12 @@
       <c r="M41" s="4">
         <v>95.119</v>
       </c>
-      <c r="U41" s="4">
-        <f t="shared" si="24"/>
+      <c r="V41" s="4">
+        <f t="shared" si="32"/>
         <v>112.187</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
@@ -3232,12 +3480,12 @@
       <c r="M42" s="4">
         <v>0.48</v>
       </c>
-      <c r="U42" s="4">
-        <f t="shared" si="24"/>
+      <c r="V42" s="4">
+        <f t="shared" si="32"/>
         <v>7.8769999999999998</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>49</v>
       </c>
@@ -3255,12 +3503,12 @@
       <c r="M43" s="4">
         <v>906.45100000000002</v>
       </c>
-      <c r="U43" s="4">
-        <f t="shared" si="24"/>
+      <c r="V43" s="4">
+        <f t="shared" si="32"/>
         <v>921.34900000000005</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>50</v>
       </c>
@@ -3276,86 +3524,94 @@
       <c r="M44" s="4">
         <v>84.292000000000002</v>
       </c>
-      <c r="U44" s="4">
-        <f t="shared" si="24"/>
+      <c r="V44" s="4">
+        <f t="shared" si="32"/>
         <v>71.013000000000005</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ref="C45:N45" si="27">SUM(C38:C44)+C37</f>
+        <f t="shared" ref="C45:N45" si="36">SUM(C38:C44)+C37</f>
         <v>0</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J45" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>4537.4080000000004</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>4608.884</v>
       </c>
       <c r="L45" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>4555.3230000000003</v>
       </c>
       <c r="M45" s="4">
         <f>SUM(M38:M44)+M37</f>
         <v>3704.5080000000003</v>
       </c>
-      <c r="N45" s="50">
-        <f t="shared" si="27"/>
+      <c r="N45" s="38">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="4">
+        <f t="shared" ref="Q45:S45" si="37">SUM(Q38:Q44)+Q37</f>
         <v>0</v>
       </c>
       <c r="R45" s="4">
-        <f t="shared" ref="R45:U45" si="28">SUM(R38:R44)+R37</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="S45" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="S45:V45" si="38">SUM(S38:S44)+S37</f>
         <v>0</v>
       </c>
       <c r="T45" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="4">
+        <f t="shared" si="38"/>
         <v>4537.4080000000004</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
       <c r="J46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="U46" s="4"/>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="V46" s="4"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>52</v>
       </c>
@@ -3371,12 +3627,12 @@
       <c r="M47" s="4">
         <v>71.408000000000001</v>
       </c>
-      <c r="U47" s="4">
-        <f t="shared" ref="U47:U51" si="29">J47</f>
+      <c r="V47" s="4">
+        <f t="shared" ref="V47:V51" si="39">J47</f>
         <v>64.072999999999993</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>53</v>
       </c>
@@ -3392,12 +3648,12 @@
       <c r="M48" s="4">
         <v>68.777000000000001</v>
       </c>
-      <c r="U48" s="4">
-        <f t="shared" si="29"/>
+      <c r="V48" s="4">
+        <f t="shared" si="39"/>
         <v>67.209999999999994</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>54</v>
       </c>
@@ -3413,12 +3669,12 @@
       <c r="M49" s="4">
         <v>218.62799999999999</v>
       </c>
-      <c r="U49" s="4">
-        <f t="shared" si="29"/>
+      <c r="V49" s="4">
+        <f t="shared" si="39"/>
         <v>200.71199999999999</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>55</v>
       </c>
@@ -3434,12 +3690,12 @@
       <c r="M50" s="4">
         <v>23.91</v>
       </c>
-      <c r="U50" s="4">
-        <f t="shared" si="29"/>
+      <c r="V50" s="4">
+        <f t="shared" si="39"/>
         <v>28.279</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>65</v>
       </c>
@@ -3455,81 +3711,89 @@
       <c r="M51" s="4">
         <v>44.701999999999998</v>
       </c>
-      <c r="U51" s="4">
-        <f t="shared" si="29"/>
+      <c r="V51" s="4">
+        <f t="shared" si="39"/>
         <v>18.568000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" ref="C52:N52" si="30">SUM(C47:C51)</f>
+        <f t="shared" ref="C52:N52" si="40">SUM(C47:C51)</f>
         <v>0</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="J52" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>378.84199999999998</v>
       </c>
       <c r="K52" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>408.37100000000004</v>
       </c>
       <c r="L52" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>389.29500000000002</v>
       </c>
       <c r="M52" s="4">
         <f>SUM(M47:M51)</f>
         <v>427.42500000000001</v>
       </c>
-      <c r="N52" s="50">
-        <f t="shared" si="30"/>
+      <c r="N52" s="38">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" ref="Q52:S52" si="41">SUM(Q47:Q51)</f>
         <v>0</v>
       </c>
       <c r="R52" s="1">
-        <f t="shared" ref="R52:U52" si="31">SUM(R47:R51)</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="S52" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="S52:V52" si="42">SUM(S47:S51)</f>
         <v>0</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="U52" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="U52" s="1">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="V52" s="4">
+        <f t="shared" si="42"/>
         <v>378.84199999999998</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>57</v>
       </c>
@@ -3545,12 +3809,12 @@
       <c r="M53" s="4">
         <v>45.073999999999998</v>
       </c>
-      <c r="U53" s="4">
-        <f t="shared" ref="U53:U56" si="32">J53</f>
+      <c r="V53" s="4">
+        <f t="shared" ref="V53:V56" si="43">J53</f>
         <v>80.768000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>58</v>
       </c>
@@ -3566,12 +3830,12 @@
       <c r="M54" s="4">
         <v>81.593000000000004</v>
       </c>
-      <c r="U54" s="4">
-        <f t="shared" si="32"/>
+      <c r="V54" s="4">
+        <f t="shared" si="43"/>
         <v>87.072999999999993</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
@@ -3587,12 +3851,12 @@
       <c r="M55" s="4">
         <v>76.977000000000004</v>
       </c>
-      <c r="U55" s="4">
-        <f t="shared" si="32"/>
+      <c r="V55" s="4">
+        <f t="shared" si="43"/>
         <v>89.917000000000002</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>59</v>
       </c>
@@ -3608,12 +3872,12 @@
       <c r="M56" s="4">
         <v>1.4570000000000001</v>
       </c>
-      <c r="U56" s="4">
-        <f t="shared" si="32"/>
+      <c r="V56" s="4">
+        <f t="shared" si="43"/>
         <v>1.9770000000000001</v>
       </c>
     </row>
-    <row r="57" spans="2:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="12" t="s">
         <v>60</v>
       </c>
@@ -3629,14 +3893,14 @@
       <c r="M57" s="23">
         <v>1961.402</v>
       </c>
-      <c r="N57" s="55"/>
-      <c r="U57" s="23">
-        <f t="shared" ref="U57:U58" si="33">J57</f>
+      <c r="N57" s="43"/>
+      <c r="V57" s="23">
+        <f t="shared" ref="V57:V58" si="44">J57</f>
         <v>2625.9589999999998</v>
       </c>
-      <c r="V57" s="55"/>
-    </row>
-    <row r="58" spans="2:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W57" s="43"/>
+    </row>
+    <row r="58" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="12" t="s">
         <v>61</v>
       </c>
@@ -3652,89 +3916,97 @@
       <c r="M58" s="23">
         <v>0</v>
       </c>
-      <c r="N58" s="55"/>
-      <c r="U58" s="23">
-        <f t="shared" si="33"/>
+      <c r="N58" s="43"/>
+      <c r="V58" s="23">
+        <f t="shared" si="44"/>
         <v>297.85599999999999</v>
       </c>
-      <c r="V58" s="55"/>
-    </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="W58" s="43"/>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:N59" si="34">SUM(C52:C58)</f>
+        <f t="shared" ref="C59:N59" si="45">SUM(C52:C58)</f>
         <v>0</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="J59" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>3562.3919999999998</v>
       </c>
       <c r="K59" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>3588.049</v>
       </c>
       <c r="L59" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="45"/>
         <v>3485.5810000000001</v>
       </c>
       <c r="M59" s="4">
         <f>SUM(M52:M58)</f>
         <v>2593.9279999999999</v>
       </c>
-      <c r="N59" s="50">
-        <f t="shared" si="34"/>
+      <c r="N59" s="38">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="Q59" s="1">
+        <f t="shared" ref="Q59:S59" si="46">SUM(Q52:Q58)</f>
         <v>0</v>
       </c>
       <c r="R59" s="1">
-        <f t="shared" ref="R59:U59" si="35">SUM(R52:R58)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="S59:V59" si="47">SUM(S52:S58)</f>
         <v>0</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="U59" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="U59" s="1">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="V59" s="4">
+        <f t="shared" si="47"/>
         <v>3562.3919999999998</v>
       </c>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:23" x14ac:dyDescent="0.2">
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>63</v>
       </c>
@@ -3750,11 +4022,11 @@
       <c r="M61" s="4">
         <v>1110.58</v>
       </c>
-      <c r="U61" s="4">
+      <c r="V61" s="4">
         <v>1110.58</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>64</v>
       </c>
@@ -3774,12 +4046,12 @@
         <f>M61+M59</f>
         <v>3704.5079999999998</v>
       </c>
-      <c r="U62" s="4">
-        <f>U61+U59</f>
+      <c r="V62" s="4">
+        <f>V61+V59</f>
         <v>4672.9719999999998</v>
       </c>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>67</v>
       </c>
@@ -3788,48 +4060,48 @@
         <v>975.01600000000053</v>
       </c>
       <c r="K64" s="4">
-        <f t="shared" ref="K64:L64" si="36">K45-K59</f>
+        <f t="shared" ref="K64" si="48">K45-K59</f>
         <v>1020.835</v>
       </c>
       <c r="L64" s="4">
-        <f t="shared" ref="L64:M64" si="37">L45-L59</f>
+        <f t="shared" ref="L64" si="49">L45-L59</f>
         <v>1069.7420000000002</v>
       </c>
       <c r="M64" s="4">
         <f>M45-M59</f>
         <v>1110.5800000000004</v>
       </c>
-      <c r="U64" s="4">
-        <f>U45-U59</f>
+      <c r="V64" s="4">
+        <f>V45-V59</f>
         <v>975.01600000000053</v>
       </c>
     </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" ref="J65:K65" si="38">J64/J20</f>
+        <f t="shared" ref="J65:K65" si="50">J64/J20</f>
         <v>8.0992158426368999</v>
       </c>
       <c r="K65" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="50"/>
         <v>8.4566413174942436</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" ref="L65" si="39">L64/L20</f>
+        <f t="shared" ref="L65" si="51">L64/L20</f>
         <v>8.8321568044650327</v>
       </c>
       <c r="M65" s="1">
         <f>M64/M20</f>
         <v>9.1666804232629584</v>
       </c>
-      <c r="U65" s="1">
-        <f>U64/U20</f>
+      <c r="V65" s="1">
+        <f>V64/V20</f>
         <v>8.0992158426368999</v>
       </c>
     </row>
-    <row r="67" spans="2:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="31" t="s">
         <v>4</v>
       </c>
@@ -3838,25 +4110,25 @@
         <v>506.49099999999999</v>
       </c>
       <c r="K67" s="32">
-        <f t="shared" ref="K67:L67" si="40">+K32</f>
+        <f t="shared" ref="K67" si="52">+K32</f>
         <v>598.50800000000004</v>
       </c>
       <c r="L67" s="32">
-        <f t="shared" ref="L67:M67" si="41">+L32</f>
+        <f t="shared" ref="L67" si="53">+L32</f>
         <v>587.86099999999999</v>
       </c>
       <c r="M67" s="32">
         <f>+M32</f>
         <v>91.644999999999996</v>
       </c>
-      <c r="N67" s="50"/>
-      <c r="U67" s="32">
-        <f>+U32</f>
+      <c r="N67" s="38"/>
+      <c r="V67" s="32">
+        <f>+V32</f>
         <v>506.49099999999999</v>
       </c>
-      <c r="V67" s="50"/>
-    </row>
-    <row r="68" spans="2:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W67" s="38"/>
+    </row>
+    <row r="68" spans="2:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="31" t="s">
         <v>5</v>
       </c>
@@ -3865,25 +4137,25 @@
         <v>2923.8149999999996</v>
       </c>
       <c r="K68" s="32">
-        <f t="shared" ref="K68:L68" si="42">K57+K58</f>
+        <f t="shared" ref="K68" si="54">K57+K58</f>
         <v>2931.1970000000001</v>
       </c>
       <c r="L68" s="32">
-        <f t="shared" ref="L68:M68" si="43">L57+L58</f>
+        <f t="shared" ref="L68" si="55">L57+L58</f>
         <v>2852.4280000000003</v>
       </c>
       <c r="M68" s="32">
         <f>M57+M58</f>
         <v>1961.402</v>
       </c>
-      <c r="N68" s="50"/>
-      <c r="U68" s="32">
-        <f>U57+U58</f>
+      <c r="N68" s="38"/>
+      <c r="V68" s="32">
+        <f>V57+V58</f>
         <v>2923.8149999999996</v>
       </c>
-      <c r="V68" s="50"/>
-    </row>
-    <row r="69" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="W68" s="38"/>
+    </row>
+    <row r="69" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
@@ -3892,23 +4164,23 @@
         <v>-2417.3239999999996</v>
       </c>
       <c r="K69" s="4">
-        <f t="shared" ref="K69" si="44">K67-K68</f>
+        <f t="shared" ref="K69" si="56">K67-K68</f>
         <v>-2332.6890000000003</v>
       </c>
       <c r="L69" s="4">
-        <f t="shared" ref="L69" si="45">L67-L68</f>
+        <f t="shared" ref="L69" si="57">L67-L68</f>
         <v>-2264.5670000000005</v>
       </c>
       <c r="M69" s="4">
         <f>M67-M68</f>
         <v>-1869.7570000000001</v>
       </c>
-      <c r="U69" s="4">
-        <f>U67-U68</f>
+      <c r="V69" s="4">
+        <f>V67-V68</f>
         <v>-2417.3239999999996</v>
       </c>
     </row>
-    <row r="71" spans="2:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:23" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="29" t="s">
         <v>90</v>
       </c>
@@ -3924,202 +4196,202 @@
       <c r="M71" s="29">
         <v>7.7</v>
       </c>
-      <c r="N71" s="59"/>
-      <c r="U71" s="29">
+      <c r="N71" s="47"/>
+      <c r="V71" s="29">
         <v>7.75</v>
       </c>
-      <c r="V71" s="59"/>
-    </row>
-    <row r="72" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W71" s="47"/>
+    </row>
+    <row r="72" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" ref="J72:L72" si="46">J71*J20</f>
+        <f t="shared" ref="J72:L72" si="58">J71*J20</f>
         <v>932.976</v>
       </c>
       <c r="K72" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v>797.91953999999998</v>
       </c>
       <c r="L72" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v>799.3854</v>
       </c>
       <c r="M72" s="4">
         <f>M71*M20</f>
         <v>932.88580000000002</v>
       </c>
-      <c r="N72" s="57"/>
-      <c r="U72" s="4">
-        <f>U71*U20</f>
+      <c r="N72" s="45"/>
+      <c r="V72" s="4">
+        <f>V71*V20</f>
         <v>932.976</v>
       </c>
-      <c r="V72" s="57"/>
-    </row>
-    <row r="73" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W72" s="45"/>
+    </row>
+    <row r="73" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" ref="J73:L73" si="47">J72-J69</f>
+        <f t="shared" ref="J73:L73" si="59">J72-J69</f>
         <v>3350.2999999999997</v>
       </c>
       <c r="K73" s="4">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>3130.6085400000002</v>
       </c>
       <c r="L73" s="4">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>3063.9524000000006</v>
       </c>
       <c r="M73" s="4">
         <f>M72-M69</f>
         <v>2802.6428000000001</v>
       </c>
-      <c r="N73" s="57"/>
-      <c r="U73" s="4">
-        <f>U72-U69</f>
+      <c r="N73" s="45"/>
+      <c r="V73" s="4">
+        <f>V72-V69</f>
         <v>3350.2999999999997</v>
       </c>
-      <c r="V73" s="57"/>
-    </row>
-    <row r="75" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="W73" s="45"/>
+    </row>
+    <row r="75" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>92</v>
       </c>
       <c r="J75" s="35">
-        <f t="shared" ref="J75:M75" si="48">J71/J65</f>
+        <f t="shared" ref="J75:L75" si="60">J71/J65</f>
         <v>0.95688275884703378</v>
       </c>
       <c r="K75" s="35">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0.78163419161764625</v>
       </c>
       <c r="L75" s="35">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0.74726934157955816</v>
       </c>
       <c r="M75" s="35">
         <f>M71/M65</f>
         <v>0.83999873939743164</v>
       </c>
-      <c r="U75" s="35">
-        <f>U71/U65</f>
+      <c r="V75" s="35">
+        <f>V71/V65</f>
         <v>0.95688275884703378</v>
       </c>
     </row>
-    <row r="76" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>93</v>
       </c>
       <c r="J76" s="35">
-        <f t="shared" ref="J76:L76" si="49">J72/SUM(G4:J4)</f>
+        <f t="shared" ref="J76:L76" si="61">J72/SUM(G4:J4)</f>
         <v>0.41344103461295073</v>
       </c>
       <c r="K76" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0.35758375384284447</v>
       </c>
       <c r="L76" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0.35462390281512812</v>
       </c>
       <c r="M76" s="35">
         <f>M72/SUM(J4:M4)</f>
         <v>0.40322106307789124</v>
       </c>
-      <c r="U76" s="35">
-        <f>U72/U4</f>
+      <c r="V76" s="35">
+        <f>V72/V4</f>
         <v>0.41344103461295073</v>
       </c>
     </row>
-    <row r="77" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>94</v>
       </c>
       <c r="J77" s="35">
-        <f t="shared" ref="J77:L77" si="50">J73/SUM(G4:J4)</f>
+        <f t="shared" ref="J77:L77" si="62">J73/SUM(G4:J4)</f>
         <v>1.4846593034159172</v>
       </c>
       <c r="K77" s="35">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>1.4029669627412142</v>
       </c>
       <c r="L77" s="35">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>1.3592326781647235</v>
       </c>
       <c r="M77" s="35">
         <f>M73/SUM(J4:M4)</f>
         <v>1.2113857979654077</v>
       </c>
-      <c r="U77" s="35">
-        <f>U73/U4</f>
+      <c r="V77" s="35">
+        <f>V73/V4</f>
         <v>1.4846593034159172</v>
       </c>
     </row>
-    <row r="78" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>95</v>
       </c>
       <c r="J78" s="35">
-        <f t="shared" ref="J78:L78" si="51">J71/SUM(G19:J19)</f>
+        <f t="shared" ref="J78:L78" si="63">J71/SUM(G19:J19)</f>
         <v>12.036038427539941</v>
       </c>
       <c r="K78" s="35">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>12.254705920751697</v>
       </c>
       <c r="L78" s="35">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>10.401043299477836</v>
       </c>
       <c r="M78" s="35">
         <f>M71/SUM(J19:M19)</f>
         <v>11.613987314778132</v>
       </c>
-      <c r="U78" s="35">
-        <f>U71/U19</f>
+      <c r="V78" s="35">
+        <f>V71/V19</f>
         <v>12.051150895140667</v>
       </c>
     </row>
-    <row r="79" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>96</v>
       </c>
       <c r="J79" s="35">
-        <f t="shared" ref="J79:L79" si="52">J73/SUM(G18:J18)</f>
+        <f t="shared" ref="J79:L79" si="64">J73/SUM(G18:J18)</f>
         <v>43.275465653982245</v>
       </c>
       <c r="K79" s="35">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>48.094396325257655</v>
       </c>
       <c r="L79" s="35">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>39.863551085726115</v>
       </c>
       <c r="M79" s="35">
         <f>M73/SUM(J18:M18)</f>
         <v>34.820629162111075</v>
       </c>
-      <c r="U79" s="35">
-        <f>U73/U18</f>
+      <c r="V79" s="35">
+        <f>V73/V18</f>
         <v>43.275465653982288</v>
       </c>
     </row>
-    <row r="80" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B82" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>124</v>
       </c>
@@ -4130,16 +4402,16 @@
         <f>91.852-K84</f>
         <v>53.673000000000002</v>
       </c>
-      <c r="M84" s="62">
+      <c r="M84" s="4">
         <f>130.164-SUM(K84:L84)</f>
         <v>38.311999999999983</v>
       </c>
     </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.2">
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>125</v>
       </c>
@@ -4153,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>126</v>
       </c>
@@ -4167,7 +4439,7 @@
         <v>1.647</v>
       </c>
     </row>
-    <row r="88" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>127</v>
       </c>
@@ -4181,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
         <v>132</v>
       </c>
@@ -4195,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>128</v>
       </c>
@@ -4211,11 +4483,11 @@
         <v>-4.6489999999999991</v>
       </c>
     </row>
-    <row r="91" spans="2:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="I91" s="63"/>
+      <c r="I91" s="50"/>
       <c r="K91" s="23">
         <v>-13.773</v>
       </c>
@@ -4227,10 +4499,10 @@
         <f>-72.233-SUM(K91:L91)</f>
         <v>-36.173000000000002</v>
       </c>
-      <c r="N91" s="55"/>
-      <c r="V91" s="55"/>
-    </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="N91" s="43"/>
+      <c r="W91" s="43"/>
+    </row>
+    <row r="92" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="s">
         <v>130</v>
       </c>
@@ -4248,10 +4520,10 @@
         <v>-39.174999999999997</v>
       </c>
     </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:23" x14ac:dyDescent="0.2">
       <c r="K93" s="4"/>
     </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
         <v>131</v>
       </c>
@@ -4266,6 +4538,11 @@
       <c r="M94" s="4">
         <f>M84-(M91)</f>
         <v>74.484999999999985</v>
+      </c>
+    </row>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B95" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4273,13 +4550,14 @@
     <hyperlink ref="M1" r:id="rId1" xr:uid="{5301AE79-155C-3744-B394-4365D45C3277}"/>
     <hyperlink ref="L1" r:id="rId2" xr:uid="{34F33EA4-D4D7-4828-A519-50670A6B56E3}"/>
     <hyperlink ref="K1" r:id="rId3" xr:uid="{D5F8DE4B-2DC9-44DD-979A-12E46C2F4C2E}"/>
-    <hyperlink ref="U1" r:id="rId4" xr:uid="{A21AFD3C-6C1E-4680-B500-57B3A4AFA330}"/>
+    <hyperlink ref="V1" r:id="rId4" xr:uid="{A21AFD3C-6C1E-4680-B500-57B3A4AFA330}"/>
+    <hyperlink ref="S1" r:id="rId5" xr:uid="{E1B3A1EF-D1AE-4EF6-89B9-14B01909731B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
   <ignoredErrors>
-    <ignoredError sqref="J8 J13:J18 U37:U59" formula="1"/>
+    <ignoredError sqref="J8 J13:J18 V37:V59" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$GEO FY22 and Q422 results
</commit_message>
<xml_diff>
--- a/$GEO.xlsx
+++ b/$GEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA08432-3388-43B8-A148-874E8A49B2B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A078CECC-DC23-40F9-9827-7D14AAF7007B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33000" windowHeight="18900" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33000" windowHeight="18900" activeTab="1" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="136">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>The Big Short's Michael Burry sells all of his portfolio except The GEO Group with a large stake</t>
-  </si>
-  <si>
-    <t>(Projected)</t>
   </si>
   <si>
     <t>FY18</t>
@@ -545,7 +542,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,12 +564,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -741,27 +732,26 @@
     <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -786,22 +776,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -890,23 +882,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2">
+        <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E118ACDD-1515-F3F9-1175-2348C9F6D0B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FEC8474-CB3F-4F5D-BF85-5A2CEEB90D79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -914,8 +906,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9197975" y="0"/>
-          <a:ext cx="0" cy="16802100"/>
+          <a:off x="15265400" y="0"/>
+          <a:ext cx="0" cy="16897350"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -940,23 +932,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
+        <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FEC8474-CB3F-4F5D-BF85-5A2CEEB90D79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEE033E-4EEC-4DA8-AB7C-FF26086F86AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -964,7 +956,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14065250" y="0"/>
+          <a:off x="9788525" y="0"/>
           <a:ext cx="0" cy="16897350"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1290,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F7E03D-6822-49B4-89BA-170833748021}">
   <dimension ref="A2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1311,24 +1303,24 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="G5" s="51" t="s">
+      <c r="B5" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="G5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
       <c r="S5" s="1" t="s">
         <v>100</v>
       </c>
@@ -1338,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>12.04</v>
+        <v>10.5</v>
       </c>
       <c r="D6" s="33"/>
       <c r="G6" s="6"/>
@@ -1360,9 +1352,9 @@
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <f>'Financial Model'!M20</f>
-        <v>121.154</v>
+      <c r="C7" s="4">
+        <f>'Financial Model'!N20</f>
+        <v>121.16500000000001</v>
       </c>
       <c r="D7" s="33" t="str">
         <f>$C$28</f>
@@ -1389,7 +1381,7 @@
       </c>
       <c r="C8" s="4">
         <f>C6*C7</f>
-        <v>1458.6941599999998</v>
+        <v>1272.2325000000001</v>
       </c>
       <c r="D8" s="33"/>
       <c r="G8" s="6"/>
@@ -1412,8 +1404,8 @@
         <v>4</v>
       </c>
       <c r="C9" s="4">
-        <f>'Financial Model'!M67</f>
-        <v>91.644999999999996</v>
+        <f>'Financial Model'!N67</f>
+        <v>95.072999999999993</v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$28</f>
@@ -1436,8 +1428,8 @@
         <v>5</v>
       </c>
       <c r="C10" s="4">
-        <f>'Financial Model'!M68</f>
-        <v>1961.402</v>
+        <f>'Financial Model'!N68</f>
+        <v>1933.145</v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" si="0"/>
@@ -1461,7 +1453,7 @@
       </c>
       <c r="C11" s="4">
         <f>C9-C10</f>
-        <v>-1869.7570000000001</v>
+        <v>-1838.0719999999999</v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" si="0"/>
@@ -1489,7 +1481,7 @@
       </c>
       <c r="C12" s="5">
         <f>C8-C11</f>
-        <v>3328.4511599999996</v>
+        <v>3110.3045000000002</v>
       </c>
       <c r="D12" s="34"/>
       <c r="G12" s="6"/>
@@ -1517,7 +1509,7 @@
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
       <c r="S13" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
@@ -1532,16 +1524,16 @@
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
-      <c r="S14" s="64" t="s">
-        <v>136</v>
+      <c r="S14" s="41" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="G15" s="6"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -1558,10 +1550,10 @@
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="50"/>
       <c r="G16" s="6"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -1578,10 +1570,10 @@
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="50"/>
       <c r="G17" s="6"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -1598,10 +1590,10 @@
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="50"/>
       <c r="G18" s="6"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -1621,10 +1613,10 @@
       <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="60"/>
+      <c r="D19" s="43"/>
       <c r="G19" s="6"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1664,11 +1656,11 @@
       <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="G22" s="7"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -1685,36 +1677,36 @@
       <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="55"/>
+      <c r="D23" s="50"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="49">
         <v>1984</v>
       </c>
-      <c r="D24" s="55"/>
+      <c r="D24" s="50"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
@@ -1732,83 +1724,77 @@
       <c r="B29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="57"/>
+      <c r="D29" s="52"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="53"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="48"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="61">
-        <f>C6/'Financial Model'!M65</f>
-        <v>1.3134525743305294</v>
-      </c>
-      <c r="D33" s="62"/>
+      <c r="C33" s="44">
+        <f>C6/'Financial Model'!N65</f>
+        <v>1.0919625813672447</v>
+      </c>
+      <c r="D33" s="45"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="61">
-        <f>C8/SUM('Financial Model'!$J$4:$M$4)</f>
-        <v>0.63049111681270253</v>
-      </c>
-      <c r="D34" s="62"/>
+      <c r="C34" s="44">
+        <f>C8/SUM('Financial Model'!K4:N4)</f>
+        <v>0.53528760349842452</v>
+      </c>
+      <c r="D34" s="45"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="61">
-        <f>C12/SUM('Financial Model'!$J$4:$M$4)</f>
-        <v>1.4386558517002188</v>
-      </c>
-      <c r="D35" s="62"/>
+      <c r="C35" s="44">
+        <f>C12/SUM('Financial Model'!$K$4:$N$4)</f>
+        <v>1.3086502993402274</v>
+      </c>
+      <c r="D35" s="45"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="61">
-        <f>C6/SUM('Financial Model'!J19:M19)</f>
-        <v>18.160052892198532</v>
-      </c>
-      <c r="D36" s="62"/>
+      <c r="C36" s="44">
+        <f>C6/SUM('Financial Model'!K19:N19)</f>
+        <v>7.353278787633327</v>
+      </c>
+      <c r="D36" s="45"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="61">
-        <f>C12/SUM('Financial Model'!J18:M18)</f>
-        <v>41.35338385846331</v>
-      </c>
-      <c r="D37" s="62"/>
+      <c r="C37" s="44">
+        <f>C12/SUM('Financial Model'!K18:N18)</f>
+        <v>17.994344774919146</v>
+      </c>
+      <c r="D37" s="45"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C29:D29"/>
@@ -1824,6 +1810,12 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{59EB0977-29E5-6644-B546-70A523E0BB16}"/>
@@ -1838,11 +1830,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7542DCCC-3188-4401-8BD1-CCBA020F892C}">
   <dimension ref="B1:AG95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1853,9 +1845,8 @@
     <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="38"/>
-    <col min="15" max="22" width="9.140625" style="1"/>
-    <col min="23" max="23" width="9.140625" style="38"/>
+    <col min="14" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.140625" style="63"/>
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1893,59 +1884,59 @@
       <c r="M1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="20" t="s">
         <v>39</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S1" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="T1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="X1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="2:33" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -1968,8 +1959,8 @@
       <c r="M2" s="25">
         <v>44834</v>
       </c>
-      <c r="N2" s="40" t="s">
-        <v>105</v>
+      <c r="N2" s="25">
+        <v>44926</v>
       </c>
       <c r="Q2" s="25">
         <v>42735</v>
@@ -1984,12 +1975,15 @@
         <v>43830</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V2" s="25">
         <v>44561</v>
       </c>
-      <c r="W2" s="40"/>
+      <c r="W2" s="55">
+        <f>N2</f>
+        <v>44926</v>
+      </c>
     </row>
     <row r="3" spans="2:33" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
@@ -2006,13 +2000,16 @@
       <c r="M3" s="26">
         <v>45226</v>
       </c>
-      <c r="N3" s="41">
+      <c r="N3" s="26">
         <v>44971</v>
       </c>
       <c r="V3" s="26">
         <v>44985</v>
       </c>
-      <c r="W3" s="40"/>
+      <c r="W3" s="56">
+        <f>N3</f>
+        <v>44971</v>
+      </c>
     </row>
     <row r="4" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
@@ -2040,9 +2037,8 @@
       <c r="M4" s="23">
         <v>616.68299999999999</v>
       </c>
-      <c r="N4" s="42">
-        <f>M4*(1+N23)</f>
-        <v>653.68398000000002</v>
+      <c r="N4" s="23">
+        <v>620.68200000000002</v>
       </c>
       <c r="Q4" s="23">
         <v>2179.4899999999998</v>
@@ -2062,9 +2058,9 @@
       <c r="V4" s="23">
         <v>2256.6120000000001</v>
       </c>
-      <c r="W4" s="42">
+      <c r="W4" s="57">
         <f>SUM(K4:N4)</f>
-        <v>2409.7289799999999</v>
+        <v>2376.7269999999999</v>
       </c>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.2">
@@ -2093,6 +2089,9 @@
       <c r="M5" s="4">
         <v>436.21</v>
       </c>
+      <c r="N5" s="4">
+        <v>430.565</v>
+      </c>
       <c r="Q5" s="4">
         <v>1650.2809999999999</v>
       </c>
@@ -2110,6 +2109,10 @@
       </c>
       <c r="V5" s="4">
         <v>1629.046</v>
+      </c>
+      <c r="W5" s="58">
+        <f>SUM(K5:N5)</f>
+        <v>1663.7270000000001</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.2">
@@ -2126,7 +2129,7 @@
         <v>32.883000000000003</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" ref="J6:J17" si="0">V6-SUM(G6:I6)</f>
+        <f>V6-SUM(G6:I6)</f>
         <v>34.870999999999981</v>
       </c>
       <c r="K6" s="4">
@@ -2138,6 +2141,9 @@
       <c r="M6" s="4">
         <v>32.33</v>
       </c>
+      <c r="N6" s="4">
+        <v>32.640999999999998</v>
+      </c>
       <c r="Q6" s="4">
         <v>114.916</v>
       </c>
@@ -2155,6 +2161,10 @@
       </c>
       <c r="V6" s="4">
         <v>135.17699999999999</v>
+      </c>
+      <c r="W6" s="58">
+        <f t="shared" ref="W6:W17" si="0">SUM(K6:N6)</f>
+        <v>132.92500000000001</v>
       </c>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.2">
@@ -2171,7 +2181,7 @@
         <v>50.475000000000001</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="0"/>
+        <f>V7-SUM(G7:I7)</f>
         <v>50.664000000000016</v>
       </c>
       <c r="K7" s="4">
@@ -2183,6 +2193,9 @@
       <c r="M7" s="4">
         <v>50.021999999999998</v>
       </c>
+      <c r="N7" s="4">
+        <v>49.040999999999997</v>
+      </c>
       <c r="Q7" s="4">
         <v>148.709</v>
       </c>
@@ -2200,6 +2213,10 @@
       </c>
       <c r="V7" s="4">
         <v>204.30600000000001</v>
+      </c>
+      <c r="W7" s="58">
+        <f t="shared" si="0"/>
+        <v>196.91899999999998</v>
       </c>
     </row>
     <row r="8" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2250,9 +2267,12 @@
         <f>M4-M5-M6-M7</f>
         <v>98.121000000000038</v>
       </c>
-      <c r="N8" s="43"/>
+      <c r="N8" s="23">
+        <f>N4-N5-N6-N7</f>
+        <v>108.43500000000003</v>
+      </c>
       <c r="Q8" s="23">
-        <f t="shared" ref="Q8:V8" si="2">Q4-Q5-Q6-Q7</f>
+        <f t="shared" ref="Q8:W8" si="2">Q4-Q5-Q6-Q7</f>
         <v>265.58399999999983</v>
       </c>
       <c r="R8" s="23">
@@ -2275,7 +2295,10 @@
         <f t="shared" si="2"/>
         <v>288.08299999999997</v>
       </c>
-      <c r="W8" s="43"/>
+      <c r="W8" s="57">
+        <f t="shared" si="2"/>
+        <v>383.15599999999984</v>
+      </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -2291,7 +2314,7 @@
         <v>5.99</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="0"/>
+        <f>V9-SUM(G9:I9)</f>
         <v>5.8300000000000018</v>
       </c>
       <c r="K9" s="4">
@@ -2303,6 +2326,9 @@
       <c r="M9" s="4">
         <v>5.1109999999999998</v>
       </c>
+      <c r="N9" s="4">
+        <v>0.53</v>
+      </c>
       <c r="Q9" s="4">
         <v>28.495999999999999</v>
       </c>
@@ -2320,6 +2346,10 @@
       </c>
       <c r="V9" s="4">
         <v>24.007000000000001</v>
+      </c>
+      <c r="W9" s="58">
+        <f t="shared" si="0"/>
+        <v>16.831000000000003</v>
       </c>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.2">
@@ -2336,7 +2366,7 @@
         <v>32.524999999999999</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="0"/>
+        <f>V10-SUM(G10:I10)</f>
         <v>33.038000000000011</v>
       </c>
       <c r="K10" s="4">
@@ -2348,6 +2378,9 @@
       <c r="M10" s="4">
         <v>46.536999999999999</v>
       </c>
+      <c r="N10" s="4">
+        <v>53.165999999999997</v>
+      </c>
       <c r="Q10" s="4">
         <v>128.71799999999999</v>
       </c>
@@ -2365,6 +2398,10 @@
       </c>
       <c r="V10" s="4">
         <v>129.46</v>
+      </c>
+      <c r="W10" s="58">
+        <f t="shared" si="0"/>
+        <v>164.54900000000001</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.2">
@@ -2381,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="0"/>
+        <f>V11-SUM(G11:I11)</f>
         <v>9.9999999999944578E-4</v>
       </c>
       <c r="K11" s="4">
@@ -2393,6 +2430,9 @@
       <c r="M11" s="4">
         <v>-37.487000000000002</v>
       </c>
+      <c r="N11" s="4">
+        <v>-0.40799999999999997</v>
+      </c>
       <c r="Q11" s="4">
         <v>-15.885</v>
       </c>
@@ -2410,6 +2450,10 @@
       </c>
       <c r="V11" s="4">
         <v>4.6929999999999996</v>
+      </c>
+      <c r="W11" s="58">
+        <f t="shared" si="0"/>
+        <v>-37.895000000000003</v>
       </c>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.2">
@@ -2426,7 +2470,7 @@
         <v>-6.0880000000000001</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="0"/>
+        <f>V12-SUM(G12:I12)</f>
         <v>1.2079999999999984</v>
       </c>
       <c r="K12" s="4">
@@ -2438,6 +2482,9 @@
       <c r="M12" s="4">
         <v>29.279</v>
       </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
       <c r="Q12" s="4">
         <v>0</v>
       </c>
@@ -2455,6 +2502,10 @@
       </c>
       <c r="V12" s="4">
         <v>5.4989999999999997</v>
+      </c>
+      <c r="W12" s="58">
+        <f t="shared" si="0"/>
+        <v>32.332000000000001</v>
       </c>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
@@ -2505,8 +2556,12 @@
         <f>M8+M9-M10+M11+M12</f>
         <v>48.487000000000037</v>
       </c>
+      <c r="N13" s="4">
+        <f>N8+N9-N10+N11+N12</f>
+        <v>55.391000000000034</v>
+      </c>
       <c r="Q13" s="4">
-        <f t="shared" ref="Q13:V13" si="4">Q8+Q9-Q10+Q11+Q12</f>
+        <f t="shared" ref="Q13:W13" si="4">Q8+Q9-Q10+Q11+Q12</f>
         <v>149.47699999999983</v>
       </c>
       <c r="R13" s="4">
@@ -2529,6 +2584,10 @@
         <f t="shared" si="4"/>
         <v>192.82199999999997</v>
       </c>
+      <c r="W13" s="59">
+        <f t="shared" si="4"/>
+        <v>229.87499999999983</v>
+      </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
@@ -2544,7 +2603,7 @@
         <v>8.3949999999999996</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="0"/>
+        <f>V14-SUM(G14:I14)</f>
         <v>101.33600000000001</v>
       </c>
       <c r="K14" s="4">
@@ -2556,6 +2615,9 @@
       <c r="M14" s="4">
         <v>11.246</v>
       </c>
+      <c r="N14" s="4">
+        <v>14.792999999999999</v>
+      </c>
       <c r="Q14" s="4">
         <v>7.9039999999999999</v>
       </c>
@@ -2573,6 +2635,10 @@
       </c>
       <c r="V14" s="4">
         <v>122.73</v>
+      </c>
+      <c r="W14" s="58">
+        <f t="shared" si="0"/>
+        <v>62.899000000000001</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.2">
@@ -2589,7 +2655,7 @@
         <v>1.64</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="0"/>
+        <f>V15-SUM(G15:I15)</f>
         <v>1.4950000000000001</v>
       </c>
       <c r="K15" s="4">
@@ -2601,6 +2667,9 @@
       <c r="M15" s="4">
         <v>1.071</v>
       </c>
+      <c r="N15" s="4">
+        <v>0.98399999999999999</v>
+      </c>
       <c r="Q15" s="4">
         <v>6.9249999999999998</v>
       </c>
@@ -2618,6 +2687,10 @@
       </c>
       <c r="V15" s="4">
         <v>7.141</v>
+      </c>
+      <c r="W15" s="58">
+        <f t="shared" si="0"/>
+        <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="16" spans="2:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2668,9 +2741,12 @@
         <f>M13-M14+M15</f>
         <v>38.312000000000033</v>
       </c>
-      <c r="N16" s="43"/>
+      <c r="N16" s="23">
+        <f>N13-N14+N15</f>
+        <v>41.582000000000036</v>
+      </c>
       <c r="Q16" s="23">
-        <f t="shared" ref="Q16:V16" si="6">Q13-Q14+Q15</f>
+        <f t="shared" ref="Q16:W16" si="6">Q13-Q14+Q15</f>
         <v>148.49799999999985</v>
       </c>
       <c r="R16" s="23">
@@ -2693,7 +2769,10 @@
         <f t="shared" si="6"/>
         <v>77.232999999999976</v>
       </c>
-      <c r="W16" s="43"/>
+      <c r="W16" s="57">
+        <f t="shared" si="6"/>
+        <v>171.74599999999984</v>
+      </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
@@ -2709,7 +2788,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="0"/>
+        <f>V17-SUM(G17:I17)</f>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="K17" s="4">
@@ -2721,6 +2800,9 @@
       <c r="M17" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="N17" s="4">
+        <v>0.98399999999999999</v>
+      </c>
       <c r="Q17" s="4">
         <v>0.217</v>
       </c>
@@ -2738,6 +2820,10 @@
       </c>
       <c r="V17" s="4">
         <v>0.185</v>
+      </c>
+      <c r="W17" s="58">
+        <f t="shared" si="0"/>
+        <v>1.103</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
@@ -2788,8 +2874,12 @@
         <f>M16+M17</f>
         <v>38.337000000000032</v>
       </c>
+      <c r="N18" s="4">
+        <f>N16+N17</f>
+        <v>42.566000000000038</v>
+      </c>
       <c r="Q18" s="4">
-        <f t="shared" ref="Q18:V18" si="8">Q16+Q17</f>
+        <f t="shared" ref="Q18:W18" si="8">Q16+Q17</f>
         <v>148.71499999999986</v>
       </c>
       <c r="R18" s="4">
@@ -2812,13 +2902,17 @@
         <f t="shared" si="8"/>
         <v>77.417999999999978</v>
       </c>
+      <c r="W18" s="58">
+        <f t="shared" si="8"/>
+        <v>172.84899999999985</v>
+      </c>
     </row>
     <row r="19" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36" t="s">
         <v>81</v>
       </c>
       <c r="G19" s="36">
-        <f t="shared" ref="G19:M19" si="9">G18/G20</f>
+        <f t="shared" ref="G19:N19" si="9">G18/G20</f>
         <v>0.42112279415440457</v>
       </c>
       <c r="H19" s="36">
@@ -2845,7 +2939,10 @@
         <f t="shared" si="9"/>
         <v>0.31643197913399501</v>
       </c>
-      <c r="N19" s="44"/>
+      <c r="N19" s="36">
+        <f t="shared" si="9"/>
+        <v>0.35130607023480409</v>
+      </c>
       <c r="Q19" s="36">
         <f t="shared" ref="Q19:S19" si="10">Q18/Q20</f>
         <v>1.3389906811326688</v>
@@ -2870,7 +2967,10 @@
         <f>V18/V20</f>
         <v>0.64309210526315774</v>
       </c>
-      <c r="W19" s="44"/>
+      <c r="W19" s="60">
+        <f>W18/W20</f>
+        <v>1.4265588247431176</v>
+      </c>
     </row>
     <row r="20" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
@@ -2898,11 +2998,13 @@
       <c r="M20" s="4">
         <v>121.154</v>
       </c>
-      <c r="N20" s="45"/>
-      <c r="Q20" s="63">
+      <c r="N20" s="4">
+        <v>121.16500000000001</v>
+      </c>
+      <c r="Q20" s="40">
         <v>111.065</v>
       </c>
-      <c r="R20" s="63">
+      <c r="R20" s="40">
         <v>120.095</v>
       </c>
       <c r="S20" s="4">
@@ -2917,11 +3019,13 @@
       <c r="V20" s="4">
         <v>120.384</v>
       </c>
-      <c r="W20" s="45"/>
+      <c r="W20" s="58">
+        <f>N20</f>
+        <v>121.16500000000001</v>
+      </c>
     </row>
     <row r="21" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N21" s="45"/>
-      <c r="W21" s="45"/>
+      <c r="W21" s="58"/>
     </row>
     <row r="22" spans="2:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
@@ -2939,30 +3043,33 @@
         <f>M4/I4-1</f>
         <v>0.10660048772872366</v>
       </c>
-      <c r="N22" s="42"/>
+      <c r="N22" s="28">
+        <f t="shared" ref="N22" si="11">N4/J4-1</f>
+        <v>0.11325306391122369</v>
+      </c>
       <c r="R22" s="28">
-        <f t="shared" ref="R22" si="11">R4/Q4-1</f>
+        <f t="shared" ref="R22" si="12">R4/Q4-1</f>
         <v>3.8509008988341531E-2</v>
       </c>
       <c r="S22" s="28">
-        <f t="shared" ref="S22" si="12">S4/R4-1</f>
+        <f t="shared" ref="S22" si="13">S4/R4-1</f>
         <v>3.0028010709457265E-2</v>
       </c>
       <c r="T22" s="28">
-        <f t="shared" ref="T22" si="13">T4/S4-1</f>
+        <f t="shared" ref="T22" si="14">T4/S4-1</f>
         <v>6.2853598674779798E-2</v>
       </c>
       <c r="U22" s="28">
-        <f t="shared" ref="U22" si="14">U4/T4-1</f>
+        <f t="shared" ref="U22" si="15">U4/T4-1</f>
         <v>-5.1585158854879243E-2</v>
       </c>
       <c r="V22" s="28">
         <f>V4/U4-1</f>
         <v>-3.9779617701048986E-2</v>
       </c>
-      <c r="W22" s="48">
+      <c r="W22" s="61">
         <f>W4/V4-1</f>
-        <v>6.7852594952078515E-2</v>
+        <v>5.322802502158086E-2</v>
       </c>
     </row>
     <row r="23" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2970,7 +3077,7 @@
         <v>83</v>
       </c>
       <c r="H23" s="30">
-        <f t="shared" ref="H23" si="15">H4/G4-1</f>
+        <f t="shared" ref="H23" si="16">H4/G4-1</f>
         <v>-1.9011862027804693E-2</v>
       </c>
       <c r="I23" s="30">
@@ -2978,58 +3085,58 @@
         <v>-1.4399940575042458E-2</v>
       </c>
       <c r="J23" s="30">
-        <f t="shared" ref="J23:L23" si="16">J4/I4-1</f>
+        <f t="shared" ref="J23:L23" si="17">J4/I4-1</f>
         <v>4.7014321423666239E-4</v>
       </c>
       <c r="K23" s="30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1.1396512172243134E-2</v>
       </c>
       <c r="L23" s="30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.7113582553952167E-2</v>
       </c>
       <c r="M23" s="30">
         <f>M4/L4-1</f>
         <v>4.8465002881785457E-2</v>
       </c>
-      <c r="N23" s="46">
-        <v>0.06</v>
-      </c>
-      <c r="Q23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="R23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="S23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="T23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="U23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="V23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="W23" s="45"/>
+      <c r="N23" s="30">
+        <f t="shared" ref="N23" si="18">N4/M4-1</f>
+        <v>6.484693108128603E-3</v>
+      </c>
+      <c r="Q23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="R23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="S23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="T23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="U23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="V23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="W23" s="58"/>
     </row>
     <row r="24" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N24" s="45"/>
-      <c r="W24" s="45"/>
+      <c r="W24" s="58"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="30">
-        <f t="shared" ref="G26" si="17">G8/G4</f>
+        <f t="shared" ref="G26" si="19">G8/G4</f>
         <v>0.11386644505245691</v>
       </c>
       <c r="H26" s="30">
-        <f t="shared" ref="H26" si="18">H8/H4</f>
+        <f t="shared" ref="H26" si="20">H8/H4</f>
         <v>0.12807493204154791</v>
       </c>
       <c r="I26" s="30">
@@ -3037,11 +3144,11 @@
         <v>0.1328226357807698</v>
       </c>
       <c r="J26" s="30">
-        <f t="shared" ref="J26:K26" si="19">J8/J4</f>
+        <f t="shared" ref="J26:K26" si="21">J8/J4</f>
         <v>0.13634561887150509</v>
       </c>
       <c r="K26" s="30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.14791041120494927</v>
       </c>
       <c r="L26" s="30">
@@ -3052,20 +3159,24 @@
         <f>M8/M4</f>
         <v>0.15911092084588035</v>
       </c>
+      <c r="N26" s="30">
+        <f t="shared" ref="N26" si="22">N8/N4</f>
+        <v>0.17470298800351874</v>
+      </c>
       <c r="Q26" s="30">
-        <f t="shared" ref="Q26:T26" si="20">Q8/Q4</f>
+        <f t="shared" ref="Q26:S26" si="23">Q8/Q4</f>
         <v>0.12185603053925453</v>
       </c>
       <c r="R26" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.10969462141361309</v>
       </c>
       <c r="S26" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.11352688915520642</v>
       </c>
       <c r="T26" s="30">
-        <f t="shared" ref="T26" si="21">T8/T4</f>
+        <f t="shared" ref="T26" si="24">T8/T4</f>
         <v>0.12232305940219262</v>
       </c>
       <c r="U26" s="30">
@@ -3076,17 +3187,21 @@
         <f>V8/V4</f>
         <v>0.12766173360772695</v>
       </c>
+      <c r="W26" s="62">
+        <f>W8/W4</f>
+        <v>0.16121161580610641</v>
+      </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G27" s="30">
-        <f t="shared" ref="G27" si="22">G16/G4</f>
+        <f t="shared" ref="G27" si="25">G16/G4</f>
         <v>8.7586770464470221E-2</v>
       </c>
       <c r="H27" s="30">
-        <f t="shared" ref="H27" si="23">H16/H4</f>
+        <f t="shared" ref="H27" si="26">H16/H4</f>
         <v>7.4159163381492241E-2</v>
       </c>
       <c r="I27" s="30">
@@ -3094,11 +3209,11 @@
         <v>6.2161187344893218E-2</v>
       </c>
       <c r="J27" s="30">
-        <f t="shared" ref="J27:K27" si="24">J16/J4</f>
+        <f t="shared" ref="J27:K27" si="27">J16/J4</f>
         <v>-8.9360564911154017E-2</v>
       </c>
       <c r="K27" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>6.9267124468191194E-2</v>
       </c>
       <c r="L27" s="30">
@@ -3109,20 +3224,24 @@
         <f>M16/M4</f>
         <v>6.212592207017225E-2</v>
       </c>
+      <c r="N27" s="30">
+        <f t="shared" ref="N27" si="28">N16/N4</f>
+        <v>6.6994048482153554E-2</v>
+      </c>
       <c r="Q27" s="30">
-        <f t="shared" ref="Q27:T27" si="25">Q16/Q4</f>
+        <f t="shared" ref="Q27:S27" si="29">Q16/Q4</f>
         <v>6.8134288296803319E-2</v>
       </c>
       <c r="R27" s="30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>6.4514760848627367E-2</v>
       </c>
       <c r="S27" s="30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>6.2124847622830402E-2</v>
       </c>
       <c r="T27" s="30">
-        <f t="shared" ref="T27" si="26">T16/T4</f>
+        <f t="shared" ref="T27" si="30">T16/T4</f>
         <v>6.7158288275417879E-2</v>
       </c>
       <c r="U27" s="30">
@@ -3133,17 +3252,21 @@
         <f>V16/V4</f>
         <v>3.4225201319500194E-2</v>
       </c>
+      <c r="W27" s="62">
+        <f>W16/W4</f>
+        <v>7.2261559699536321E-2</v>
+      </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G28" s="30">
-        <f t="shared" ref="G28" si="27">G14/G13</f>
+        <f t="shared" ref="G28" si="31">G14/G13</f>
         <v>0.14082157749977833</v>
       </c>
       <c r="H28" s="30">
-        <f t="shared" ref="H28" si="28">H14/H13</f>
+        <f t="shared" ref="H28" si="32">H14/H13</f>
         <v>0.11238124833525712</v>
       </c>
       <c r="I28" s="30">
@@ -3151,11 +3274,11 @@
         <v>0.20279737172673659</v>
       </c>
       <c r="J28" s="30">
-        <f t="shared" ref="J28:K28" si="29">J14/J13</f>
+        <f t="shared" ref="J28:K28" si="33">J14/J13</f>
         <v>2.0259501389471963</v>
       </c>
       <c r="K28" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.32714093177430542</v>
       </c>
       <c r="L28" s="30">
@@ -3166,20 +3289,24 @@
         <f>M14/M13</f>
         <v>0.23193845773093802</v>
       </c>
+      <c r="N28" s="30">
+        <f t="shared" ref="N28" si="34">N14/N13</f>
+        <v>0.26706504666823111</v>
+      </c>
       <c r="Q28" s="30">
-        <f t="shared" ref="Q28:T28" si="30">Q14/Q13</f>
+        <f t="shared" ref="Q28:S28" si="35">Q14/Q13</f>
         <v>5.2877700248198781E-2</v>
       </c>
       <c r="R28" s="30">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.11819372503076918</v>
       </c>
       <c r="S28" s="30">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>9.4537491545400337E-2</v>
       </c>
       <c r="T28" s="30">
-        <f t="shared" ref="T28" si="31">T14/T13</f>
+        <f t="shared" ref="T28" si="36">T14/T13</f>
         <v>9.5937854767790973E-2</v>
       </c>
       <c r="U28" s="30">
@@ -3190,6 +3317,10 @@
         <f>V14/V13</f>
         <v>0.63649376108535338</v>
       </c>
+      <c r="W28" s="62">
+        <f>W14/W13</f>
+        <v>0.2736226209896685</v>
+      </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B31" s="22" t="s">
@@ -3212,12 +3343,14 @@
       <c r="M32" s="23">
         <v>91.644999999999996</v>
       </c>
-      <c r="N32" s="43"/>
+      <c r="N32" s="23">
+        <v>95.072999999999993</v>
+      </c>
       <c r="V32" s="23">
         <f>J32</f>
         <v>506.49099999999999</v>
       </c>
-      <c r="W32" s="43"/>
+      <c r="W32" s="64"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3235,6 +3368,9 @@
       <c r="M33" s="4">
         <v>0</v>
       </c>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
       <c r="V33" s="4">
         <f>J33</f>
         <v>20.161000000000001</v>
@@ -3256,8 +3392,11 @@
       <c r="M34" s="4">
         <v>383.69400000000002</v>
       </c>
+      <c r="N34" s="4">
+        <v>416.399</v>
+      </c>
       <c r="V34" s="4">
-        <f t="shared" ref="V34:V44" si="32">J34</f>
+        <f>J34</f>
         <v>365.57299999999998</v>
       </c>
     </row>
@@ -3277,8 +3416,11 @@
       <c r="M35" s="4">
         <v>0</v>
       </c>
+      <c r="N35" s="4">
+        <v>0</v>
+      </c>
       <c r="V35" s="4">
-        <f t="shared" si="32"/>
+        <f>J35</f>
         <v>6.5069999999999997</v>
       </c>
     </row>
@@ -3298,8 +3440,11 @@
       <c r="M36" s="4">
         <v>40.387999999999998</v>
       </c>
+      <c r="N36" s="4">
+        <v>43.536000000000001</v>
+      </c>
       <c r="V36" s="4">
-        <f t="shared" si="32"/>
+        <f>J36</f>
         <v>45.176000000000002</v>
       </c>
     </row>
@@ -3308,75 +3453,75 @@
         <v>45</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ref="C37:N37" si="33">SUM(C32:C36)</f>
+        <f t="shared" ref="C37:L37" si="37">SUM(C32:C36)</f>
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>943.90800000000002</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>1022.8150000000001</v>
       </c>
       <c r="L37" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>1023.413</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(M32:M36)</f>
         <v>515.72699999999998</v>
       </c>
-      <c r="N37" s="38">
-        <f t="shared" si="33"/>
-        <v>0</v>
+      <c r="N37" s="4">
+        <f>SUM(N32:N36)</f>
+        <v>555.00800000000004</v>
       </c>
       <c r="Q37" s="4">
-        <f t="shared" ref="Q37:S37" si="34">SUM(Q32:Q36)</f>
+        <f t="shared" ref="Q37:R37" si="38">SUM(Q32:Q36)</f>
         <v>0</v>
       </c>
       <c r="R37" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="S37" s="4">
-        <f t="shared" ref="S37:V37" si="35">SUM(S32:S36)</f>
+        <f t="shared" ref="S37:V37" si="39">SUM(S32:S36)</f>
         <v>0</v>
       </c>
       <c r="T37" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="U37" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="V37" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>943.90800000000002</v>
       </c>
     </row>
@@ -3396,8 +3541,11 @@
       <c r="M38" s="4">
         <v>89.76</v>
       </c>
+      <c r="N38" s="4">
+        <v>111.691</v>
+      </c>
       <c r="V38" s="4">
-        <f t="shared" si="32"/>
+        <f>J38</f>
         <v>76.158000000000001</v>
       </c>
     </row>
@@ -3417,8 +3565,11 @@
       <c r="M39" s="4">
         <v>2012.6790000000001</v>
       </c>
+      <c r="N39" s="4">
+        <v>2002.021</v>
+      </c>
       <c r="V39" s="4">
-        <f t="shared" si="32"/>
+        <f>J39</f>
         <v>2037.845</v>
       </c>
     </row>
@@ -3438,8 +3589,11 @@
       <c r="M40" s="4">
         <v>0</v>
       </c>
+      <c r="N40" s="4">
+        <v>0</v>
+      </c>
       <c r="V40" s="4">
-        <f t="shared" si="32"/>
+        <f>J40</f>
         <v>367.07100000000003</v>
       </c>
     </row>
@@ -3459,8 +3613,11 @@
       <c r="M41" s="4">
         <v>95.119</v>
       </c>
+      <c r="N41" s="4">
+        <v>90.95</v>
+      </c>
       <c r="V41" s="4">
-        <f t="shared" si="32"/>
+        <f>J41</f>
         <v>112.187</v>
       </c>
     </row>
@@ -3480,8 +3637,11 @@
       <c r="M42" s="4">
         <v>0.48</v>
       </c>
+      <c r="N42" s="4">
+        <v>0.48</v>
+      </c>
       <c r="V42" s="4">
-        <f t="shared" si="32"/>
+        <f>J42</f>
         <v>7.8769999999999998</v>
       </c>
     </row>
@@ -3503,8 +3663,11 @@
       <c r="M43" s="4">
         <v>906.45100000000002</v>
       </c>
+      <c r="N43" s="4">
+        <v>902.88699999999994</v>
+      </c>
       <c r="V43" s="4">
-        <f t="shared" si="32"/>
+        <f>J43</f>
         <v>921.34900000000005</v>
       </c>
     </row>
@@ -3524,8 +3687,12 @@
       <c r="M44" s="4">
         <v>84.292000000000002</v>
       </c>
+      <c r="N44" s="4">
+        <f>8.005+89.341</f>
+        <v>97.345999999999989</v>
+      </c>
       <c r="V44" s="4">
-        <f t="shared" si="32"/>
+        <f>J44</f>
         <v>71.013000000000005</v>
       </c>
     </row>
@@ -3534,81 +3701,82 @@
         <v>51</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ref="C45:N45" si="36">SUM(C38:C44)+C37</f>
+        <f t="shared" ref="C45:L45" si="40">SUM(C38:C44)+C37</f>
         <v>0</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="J45" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>4537.4080000000004</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>4608.884</v>
       </c>
       <c r="L45" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>4555.3230000000003</v>
       </c>
       <c r="M45" s="4">
         <f>SUM(M38:M44)+M37</f>
         <v>3704.5080000000003</v>
       </c>
-      <c r="N45" s="38">
-        <f t="shared" si="36"/>
-        <v>0</v>
+      <c r="N45" s="4">
+        <f>SUM(N38:N44)+N37</f>
+        <v>3760.3829999999998</v>
       </c>
       <c r="Q45" s="4">
-        <f t="shared" ref="Q45:S45" si="37">SUM(Q38:Q44)+Q37</f>
+        <f t="shared" ref="Q45:R45" si="41">SUM(Q38:Q44)+Q37</f>
         <v>0</v>
       </c>
       <c r="R45" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="S45" s="4">
-        <f t="shared" ref="S45:V45" si="38">SUM(S38:S44)+S37</f>
+        <f t="shared" ref="S45:V45" si="42">SUM(S38:S44)+S37</f>
         <v>0</v>
       </c>
       <c r="T45" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="V45" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>4537.4080000000004</v>
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.2">
       <c r="J46" s="4"/>
       <c r="L46" s="4"/>
+      <c r="N46" s="4"/>
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.2">
@@ -3627,8 +3795,11 @@
       <c r="M47" s="4">
         <v>71.408000000000001</v>
       </c>
+      <c r="N47" s="4">
+        <v>79.311999999999998</v>
+      </c>
       <c r="V47" s="4">
-        <f t="shared" ref="V47:V51" si="39">J47</f>
+        <f>J47</f>
         <v>64.072999999999993</v>
       </c>
     </row>
@@ -3648,8 +3819,11 @@
       <c r="M48" s="4">
         <v>68.777000000000001</v>
       </c>
+      <c r="N48" s="4">
+        <v>53.225000000000001</v>
+      </c>
       <c r="V48" s="4">
-        <f t="shared" si="39"/>
+        <f>J48</f>
         <v>67.209999999999994</v>
       </c>
     </row>
@@ -3669,8 +3843,11 @@
       <c r="M49" s="4">
         <v>218.62799999999999</v>
       </c>
+      <c r="N49" s="4">
+        <v>237.369</v>
+      </c>
       <c r="V49" s="4">
-        <f t="shared" si="39"/>
+        <f>J49</f>
         <v>200.71199999999999</v>
       </c>
     </row>
@@ -3690,8 +3867,11 @@
       <c r="M50" s="4">
         <v>23.91</v>
       </c>
+      <c r="N50" s="4">
+        <v>22.584</v>
+      </c>
       <c r="V50" s="4">
-        <f t="shared" si="39"/>
+        <f>J50</f>
         <v>28.279</v>
       </c>
     </row>
@@ -3711,8 +3891,11 @@
       <c r="M51" s="4">
         <v>44.701999999999998</v>
       </c>
+      <c r="N51" s="4">
+        <v>44.722000000000001</v>
+      </c>
       <c r="V51" s="4">
-        <f t="shared" si="39"/>
+        <f>J51</f>
         <v>18.568000000000001</v>
       </c>
     </row>
@@ -3721,75 +3904,75 @@
         <v>56</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" ref="C52:N52" si="40">SUM(C47:C51)</f>
+        <f t="shared" ref="C52:L52" si="43">SUM(C47:C51)</f>
         <v>0</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="J52" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>378.84199999999998</v>
       </c>
       <c r="K52" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>408.37100000000004</v>
       </c>
       <c r="L52" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>389.29500000000002</v>
       </c>
       <c r="M52" s="4">
         <f>SUM(M47:M51)</f>
         <v>427.42500000000001</v>
       </c>
-      <c r="N52" s="38">
-        <f t="shared" si="40"/>
-        <v>0</v>
+      <c r="N52" s="4">
+        <f>SUM(N47:N51)</f>
+        <v>437.21199999999999</v>
       </c>
       <c r="Q52" s="1">
-        <f t="shared" ref="Q52:S52" si="41">SUM(Q47:Q51)</f>
+        <f t="shared" ref="Q52:R52" si="44">SUM(Q47:Q51)</f>
         <v>0</v>
       </c>
       <c r="R52" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="S52" s="1">
-        <f t="shared" ref="S52:V52" si="42">SUM(S47:S51)</f>
+        <f t="shared" ref="S52:V52" si="45">SUM(S47:S51)</f>
         <v>0</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V52" s="4">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>378.84199999999998</v>
       </c>
     </row>
@@ -3809,8 +3992,11 @@
       <c r="M53" s="4">
         <v>45.073999999999998</v>
       </c>
+      <c r="N53" s="4">
+        <v>75.849000000000004</v>
+      </c>
       <c r="V53" s="4">
-        <f t="shared" ref="V53:V56" si="43">J53</f>
+        <f>J53</f>
         <v>80.768000000000001</v>
       </c>
     </row>
@@ -3830,8 +4016,11 @@
       <c r="M54" s="4">
         <v>81.593000000000004</v>
       </c>
+      <c r="N54" s="4">
+        <v>74.007999999999996</v>
+      </c>
       <c r="V54" s="4">
-        <f t="shared" si="43"/>
+        <f>J54</f>
         <v>87.072999999999993</v>
       </c>
     </row>
@@ -3851,8 +4040,11 @@
       <c r="M55" s="4">
         <v>76.977000000000004</v>
       </c>
+      <c r="N55" s="4">
+        <v>73.801000000000002</v>
+      </c>
       <c r="V55" s="4">
-        <f t="shared" si="43"/>
+        <f>J55</f>
         <v>89.917000000000002</v>
       </c>
     </row>
@@ -3872,8 +4064,11 @@
       <c r="M56" s="4">
         <v>1.4570000000000001</v>
       </c>
+      <c r="N56" s="4">
+        <v>1.28</v>
+      </c>
       <c r="V56" s="4">
-        <f t="shared" si="43"/>
+        <f>J56</f>
         <v>1.9770000000000001</v>
       </c>
     </row>
@@ -3893,12 +4088,14 @@
       <c r="M57" s="23">
         <v>1961.402</v>
       </c>
-      <c r="N57" s="43"/>
+      <c r="N57" s="23">
+        <v>1933.145</v>
+      </c>
       <c r="V57" s="23">
-        <f t="shared" ref="V57:V58" si="44">J57</f>
+        <f>J57</f>
         <v>2625.9589999999998</v>
       </c>
-      <c r="W57" s="43"/>
+      <c r="W57" s="64"/>
     </row>
     <row r="58" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="12" t="s">
@@ -3916,87 +4113,89 @@
       <c r="M58" s="23">
         <v>0</v>
       </c>
-      <c r="N58" s="43"/>
+      <c r="N58" s="23">
+        <v>0</v>
+      </c>
       <c r="V58" s="23">
-        <f t="shared" si="44"/>
+        <f>J58</f>
         <v>297.85599999999999</v>
       </c>
-      <c r="W58" s="43"/>
+      <c r="W58" s="64"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:N59" si="45">SUM(C52:C58)</f>
+        <f t="shared" ref="C59:L59" si="46">SUM(C52:C58)</f>
         <v>0</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="J59" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>3562.3919999999998</v>
       </c>
       <c r="K59" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>3588.049</v>
       </c>
       <c r="L59" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>3485.5810000000001</v>
       </c>
       <c r="M59" s="4">
         <f>SUM(M52:M58)</f>
         <v>2593.9279999999999</v>
       </c>
-      <c r="N59" s="38">
-        <f t="shared" si="45"/>
-        <v>0</v>
+      <c r="N59" s="4">
+        <f>SUM(N52:N58)</f>
+        <v>2595.2950000000001</v>
       </c>
       <c r="Q59" s="1">
-        <f t="shared" ref="Q59:S59" si="46">SUM(Q52:Q58)</f>
+        <f t="shared" ref="Q59:R59" si="47">SUM(Q52:Q58)</f>
         <v>0</v>
       </c>
       <c r="R59" s="1">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <f t="shared" ref="S59:V59" si="47">SUM(S52:S58)</f>
+        <f t="shared" ref="S59:V59" si="48">SUM(S52:S58)</f>
         <v>0</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="V59" s="4">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>3562.3919999999998</v>
       </c>
     </row>
@@ -4005,6 +4204,7 @@
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
@@ -4022,6 +4222,9 @@
       <c r="M61" s="4">
         <v>1110.58</v>
       </c>
+      <c r="N61" s="4">
+        <v>1165.088</v>
+      </c>
       <c r="V61" s="4">
         <v>1110.58</v>
       </c>
@@ -4046,6 +4249,10 @@
         <f>M61+M59</f>
         <v>3704.5079999999998</v>
       </c>
+      <c r="N62" s="4">
+        <f>N61+N59</f>
+        <v>3760.3829999999998</v>
+      </c>
       <c r="V62" s="4">
         <f>V61+V59</f>
         <v>4672.9719999999998</v>
@@ -4060,17 +4267,21 @@
         <v>975.01600000000053</v>
       </c>
       <c r="K64" s="4">
-        <f t="shared" ref="K64" si="48">K45-K59</f>
+        <f t="shared" ref="K64" si="49">K45-K59</f>
         <v>1020.835</v>
       </c>
       <c r="L64" s="4">
-        <f t="shared" ref="L64" si="49">L45-L59</f>
+        <f t="shared" ref="L64" si="50">L45-L59</f>
         <v>1069.7420000000002</v>
       </c>
       <c r="M64" s="4">
         <f>M45-M59</f>
         <v>1110.5800000000004</v>
       </c>
+      <c r="N64" s="4">
+        <f t="shared" ref="N64" si="51">N45-N59</f>
+        <v>1165.0879999999997</v>
+      </c>
       <c r="V64" s="4">
         <f>V45-V59</f>
         <v>975.01600000000053</v>
@@ -4081,21 +4292,25 @@
         <v>68</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" ref="J65:K65" si="50">J64/J20</f>
+        <f t="shared" ref="J65:K65" si="52">J64/J20</f>
         <v>8.0992158426368999</v>
       </c>
       <c r="K65" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>8.4566413174942436</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" ref="L65" si="51">L64/L20</f>
+        <f t="shared" ref="L65" si="53">L64/L20</f>
         <v>8.8321568044650327</v>
       </c>
       <c r="M65" s="1">
         <f>M64/M20</f>
         <v>9.1666804232629584</v>
       </c>
+      <c r="N65" s="1">
+        <f t="shared" ref="N65" si="54">N64/N20</f>
+        <v>9.6157141088598159</v>
+      </c>
       <c r="V65" s="1">
         <f>V64/V20</f>
         <v>8.0992158426368999</v>
@@ -4110,23 +4325,26 @@
         <v>506.49099999999999</v>
       </c>
       <c r="K67" s="32">
-        <f t="shared" ref="K67" si="52">+K32</f>
+        <f t="shared" ref="K67" si="55">+K32</f>
         <v>598.50800000000004</v>
       </c>
       <c r="L67" s="32">
-        <f t="shared" ref="L67" si="53">+L32</f>
+        <f t="shared" ref="L67" si="56">+L32</f>
         <v>587.86099999999999</v>
       </c>
       <c r="M67" s="32">
         <f>+M32</f>
         <v>91.644999999999996</v>
       </c>
-      <c r="N67" s="38"/>
+      <c r="N67" s="32">
+        <f t="shared" ref="N67" si="57">+N32</f>
+        <v>95.072999999999993</v>
+      </c>
       <c r="V67" s="32">
         <f>+V32</f>
         <v>506.49099999999999</v>
       </c>
-      <c r="W67" s="38"/>
+      <c r="W67" s="63"/>
     </row>
     <row r="68" spans="2:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="31" t="s">
@@ -4137,23 +4355,26 @@
         <v>2923.8149999999996</v>
       </c>
       <c r="K68" s="32">
-        <f t="shared" ref="K68" si="54">K57+K58</f>
+        <f t="shared" ref="K68" si="58">K57+K58</f>
         <v>2931.1970000000001</v>
       </c>
       <c r="L68" s="32">
-        <f t="shared" ref="L68" si="55">L57+L58</f>
+        <f t="shared" ref="L68" si="59">L57+L58</f>
         <v>2852.4280000000003</v>
       </c>
       <c r="M68" s="32">
         <f>M57+M58</f>
         <v>1961.402</v>
       </c>
-      <c r="N68" s="38"/>
+      <c r="N68" s="32">
+        <f t="shared" ref="N68" si="60">N57+N58</f>
+        <v>1933.145</v>
+      </c>
       <c r="V68" s="32">
         <f>V57+V58</f>
         <v>2923.8149999999996</v>
       </c>
-      <c r="W68" s="38"/>
+      <c r="W68" s="63"/>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
@@ -4164,17 +4385,21 @@
         <v>-2417.3239999999996</v>
       </c>
       <c r="K69" s="4">
-        <f t="shared" ref="K69" si="56">K67-K68</f>
+        <f t="shared" ref="K69" si="61">K67-K68</f>
         <v>-2332.6890000000003</v>
       </c>
       <c r="L69" s="4">
-        <f t="shared" ref="L69" si="57">L67-L68</f>
+        <f t="shared" ref="L69" si="62">L67-L68</f>
         <v>-2264.5670000000005</v>
       </c>
       <c r="M69" s="4">
         <f>M67-M68</f>
         <v>-1869.7570000000001</v>
       </c>
+      <c r="N69" s="4">
+        <f t="shared" ref="N69" si="63">N67-N68</f>
+        <v>-1838.0719999999999</v>
+      </c>
       <c r="V69" s="4">
         <f>V67-V68</f>
         <v>-2417.3239999999996</v>
@@ -4196,86 +4421,98 @@
       <c r="M71" s="29">
         <v>7.7</v>
       </c>
-      <c r="N71" s="47"/>
+      <c r="N71" s="29">
+        <v>10.95</v>
+      </c>
       <c r="V71" s="29">
         <v>7.75</v>
       </c>
-      <c r="W71" s="47"/>
+      <c r="W71" s="65"/>
     </row>
     <row r="72" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" ref="J72:L72" si="58">J71*J20</f>
+        <f t="shared" ref="J72:L72" si="64">J71*J20</f>
         <v>932.976</v>
       </c>
       <c r="K72" s="4">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>797.91953999999998</v>
       </c>
       <c r="L72" s="4">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>799.3854</v>
       </c>
       <c r="M72" s="4">
         <f>M71*M20</f>
         <v>932.88580000000002</v>
       </c>
-      <c r="N72" s="45"/>
+      <c r="N72" s="4">
+        <f t="shared" ref="N72" si="65">N71*N20</f>
+        <v>1326.75675</v>
+      </c>
       <c r="V72" s="4">
         <f>V71*V20</f>
         <v>932.976</v>
       </c>
-      <c r="W72" s="45"/>
+      <c r="W72" s="58"/>
     </row>
     <row r="73" spans="2:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" ref="J73:L73" si="59">J72-J69</f>
+        <f t="shared" ref="J73:L73" si="66">J72-J69</f>
         <v>3350.2999999999997</v>
       </c>
       <c r="K73" s="4">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>3130.6085400000002</v>
       </c>
       <c r="L73" s="4">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>3063.9524000000006</v>
       </c>
       <c r="M73" s="4">
         <f>M72-M69</f>
         <v>2802.6428000000001</v>
       </c>
-      <c r="N73" s="45"/>
+      <c r="N73" s="4">
+        <f t="shared" ref="N73" si="67">N72-N69</f>
+        <v>3164.8287499999997</v>
+      </c>
       <c r="V73" s="4">
         <f>V72-V69</f>
         <v>3350.2999999999997</v>
       </c>
-      <c r="W73" s="45"/>
+      <c r="W73" s="58"/>
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>92</v>
       </c>
       <c r="J75" s="35">
-        <f t="shared" ref="J75:L75" si="60">J71/J65</f>
+        <f t="shared" ref="J75:L75" si="68">J71/J65</f>
         <v>0.95688275884703378</v>
       </c>
       <c r="K75" s="35">
-        <f t="shared" si="60"/>
+        <f t="shared" si="68"/>
         <v>0.78163419161764625</v>
       </c>
       <c r="L75" s="35">
-        <f t="shared" si="60"/>
+        <f t="shared" si="68"/>
         <v>0.74726934157955816</v>
       </c>
       <c r="M75" s="35">
         <f>M71/M65</f>
         <v>0.83999873939743164</v>
       </c>
+      <c r="N75" s="35">
+        <f t="shared" ref="N75" si="69">N71/N65</f>
+        <v>1.1387609777115553</v>
+      </c>
       <c r="V75" s="35">
         <f>V71/V65</f>
         <v>0.95688275884703378</v>
@@ -4286,21 +4523,25 @@
         <v>93</v>
       </c>
       <c r="J76" s="35">
-        <f t="shared" ref="J76:L76" si="61">J72/SUM(G4:J4)</f>
+        <f t="shared" ref="J76:L76" si="70">J72/SUM(G4:J4)</f>
         <v>0.41344103461295073</v>
       </c>
       <c r="K76" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>0.35758375384284447</v>
       </c>
       <c r="L76" s="35">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>0.35462390281512812</v>
       </c>
       <c r="M76" s="35">
         <f>M72/SUM(J4:M4)</f>
         <v>0.40322106307789124</v>
       </c>
+      <c r="N76" s="35">
+        <f t="shared" ref="N76" si="71">N72/SUM(K4:N4)</f>
+        <v>0.55822850079121422</v>
+      </c>
       <c r="V76" s="35">
         <f>V72/V4</f>
         <v>0.41344103461295073</v>
@@ -4311,21 +4552,25 @@
         <v>94</v>
       </c>
       <c r="J77" s="35">
-        <f t="shared" ref="J77:L77" si="62">J73/SUM(G4:J4)</f>
+        <f t="shared" ref="J77:L77" si="72">J73/SUM(G4:J4)</f>
         <v>1.4846593034159172</v>
       </c>
       <c r="K77" s="35">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>1.4029669627412142</v>
       </c>
       <c r="L77" s="35">
-        <f t="shared" si="62"/>
+        <f t="shared" si="72"/>
         <v>1.3592326781647235</v>
       </c>
       <c r="M77" s="35">
         <f>M73/SUM(J4:M4)</f>
         <v>1.2113857979654077</v>
       </c>
+      <c r="N77" s="35">
+        <f t="shared" ref="N77" si="73">N73/SUM(K4:N4)</f>
+        <v>1.3315911966330167</v>
+      </c>
       <c r="V77" s="35">
         <f>V73/V4</f>
         <v>1.4846593034159172</v>
@@ -4336,21 +4581,25 @@
         <v>95</v>
       </c>
       <c r="J78" s="35">
-        <f t="shared" ref="J78:L78" si="63">J71/SUM(G19:J19)</f>
+        <f t="shared" ref="J78:L78" si="74">J71/SUM(G19:J19)</f>
         <v>12.036038427539941</v>
       </c>
       <c r="K78" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="74"/>
         <v>12.254705920751697</v>
       </c>
       <c r="L78" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="74"/>
         <v>10.401043299477836</v>
       </c>
       <c r="M78" s="35">
         <f>M71/SUM(J19:M19)</f>
         <v>11.613987314778132</v>
       </c>
+      <c r="N78" s="35">
+        <f t="shared" ref="N78" si="75">N71/SUM(K19:N19)</f>
+        <v>7.668419307103326</v>
+      </c>
       <c r="V78" s="35">
         <f>V71/V19</f>
         <v>12.051150895140667</v>
@@ -4361,21 +4610,25 @@
         <v>96</v>
       </c>
       <c r="J79" s="35">
-        <f t="shared" ref="J79:L79" si="64">J73/SUM(G18:J18)</f>
+        <f t="shared" ref="J79:L79" si="76">J73/SUM(G18:J18)</f>
         <v>43.275465653982245</v>
       </c>
       <c r="K79" s="35">
-        <f t="shared" si="64"/>
+        <f t="shared" si="76"/>
         <v>48.094396325257655</v>
       </c>
       <c r="L79" s="35">
-        <f t="shared" si="64"/>
+        <f t="shared" si="76"/>
         <v>39.863551085726115</v>
       </c>
       <c r="M79" s="35">
         <f>M73/SUM(J18:M18)</f>
         <v>34.820629162111075</v>
       </c>
+      <c r="N79" s="35">
+        <f t="shared" ref="N79" si="77">N73/SUM(K18:N18)</f>
+        <v>18.309789180151455</v>
+      </c>
       <c r="V79" s="35">
         <f>V73/V18</f>
         <v>43.275465653982288</v>
@@ -4393,7 +4646,7 @@
     </row>
     <row r="84" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K84" s="4">
         <v>38.179000000000002</v>
@@ -4406,6 +4659,7 @@
         <f>130.164-SUM(K84:L84)</f>
         <v>38.311999999999983</v>
       </c>
+      <c r="N84" s="4"/>
     </row>
     <row r="85" spans="2:23" x14ac:dyDescent="0.2">
       <c r="K85" s="4"/>
@@ -4413,7 +4667,7 @@
     </row>
     <row r="86" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K86" s="4">
         <v>0</v>
@@ -4427,7 +4681,7 @@
     </row>
     <row r="87" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K87" s="4">
         <v>4.1000000000000002E-2</v>
@@ -4441,7 +4695,7 @@
     </row>
     <row r="88" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K88" s="4">
         <v>0</v>
@@ -4455,7 +4709,7 @@
     </row>
     <row r="89" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K89" s="4">
         <v>0</v>
@@ -4469,7 +4723,7 @@
     </row>
     <row r="90" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K90" s="4">
         <v>-4.109</v>
@@ -4485,9 +4739,9 @@
     </row>
     <row r="91" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="I91" s="50"/>
+        <v>128</v>
+      </c>
+      <c r="I91" s="39"/>
       <c r="K91" s="23">
         <v>-13.773</v>
       </c>
@@ -4499,12 +4753,11 @@
         <f>-72.233-SUM(K91:L91)</f>
         <v>-36.173000000000002</v>
       </c>
-      <c r="N91" s="43"/>
-      <c r="W91" s="43"/>
+      <c r="W91" s="64"/>
     </row>
     <row r="92" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I92" s="4"/>
       <c r="K92" s="4">
@@ -4525,7 +4778,7 @@
     </row>
     <row r="94" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K94" s="4">
         <f>K84-(K91)</f>
@@ -4542,7 +4795,7 @@
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4552,12 +4805,13 @@
     <hyperlink ref="K1" r:id="rId3" xr:uid="{D5F8DE4B-2DC9-44DD-979A-12E46C2F4C2E}"/>
     <hyperlink ref="V1" r:id="rId4" xr:uid="{A21AFD3C-6C1E-4680-B500-57B3A4AFA330}"/>
     <hyperlink ref="S1" r:id="rId5" xr:uid="{E1B3A1EF-D1AE-4EF6-89B9-14B01909731B}"/>
+    <hyperlink ref="N1" r:id="rId6" xr:uid="{BFBCC226-B105-4498-8E78-0CF30EEB8CCA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId7"/>
   <ignoredErrors>
-    <ignoredError sqref="J8 J13:J18 V37:V59" formula="1"/>
+    <ignoredError sqref="J8 J13:J18 V37:V59 W8:W13 W14:W20" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>